<commit_message>
Bug fix to correct missing year's data for BCDTRtSY
</commit_message>
<xml_diff>
--- a/InputData/trans/BCDTRtSY/BAU Cargo Dist Transported Relative to Start Yr.xlsx
+++ b/InputData/trans/BCDTRtSY/BAU Cargo Dist Transported Relative to Start Yr.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Dropbox (Energy Innovation)\Documents\EPS_Models by Region\United States\Model\InputData\trans\BCDTRtSY\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Documents\eps-us\InputData\trans\BCDTRtSY\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA5E7701-C27E-4447-BDB5-AEB27358771F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="817" yWindow="23" windowWidth="17798" windowHeight="10049" xr2:uid="{577E5D68-AD55-4212-BB77-63298B94F239}"/>
+    <workbookView xWindow="818" yWindow="23" windowWidth="17798" windowHeight="10050"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -40,8 +39,7 @@
     <definedName name="ti_tbl_69" localSheetId="8">#REF!</definedName>
     <definedName name="ti_tbl_69">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="191029" iterate="1" iterateDelta="1.0000000000000001E-5"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -1753,7 +1751,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="6">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
@@ -3280,221 +3278,221 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="28" borderId="4" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="28" borderId="4" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="207">
     <cellStyle name="20% - Accent1" xfId="170" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent1 2" xfId="8" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="20% - Accent1 2 2" xfId="195" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="20% - Accent1 2" xfId="8"/>
+    <cellStyle name="20% - Accent1 2 2" xfId="195"/>
     <cellStyle name="20% - Accent2" xfId="173" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2 2" xfId="9" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
-    <cellStyle name="20% - Accent2 2 2" xfId="197" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="20% - Accent2 2" xfId="9"/>
+    <cellStyle name="20% - Accent2 2 2" xfId="197"/>
     <cellStyle name="20% - Accent3" xfId="176" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3 2" xfId="10" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
-    <cellStyle name="20% - Accent3 2 2" xfId="199" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="20% - Accent3 2" xfId="10"/>
+    <cellStyle name="20% - Accent3 2 2" xfId="199"/>
     <cellStyle name="20% - Accent4" xfId="179" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4 2" xfId="11" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
-    <cellStyle name="20% - Accent4 2 2" xfId="201" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
+    <cellStyle name="20% - Accent4 2" xfId="11"/>
+    <cellStyle name="20% - Accent4 2 2" xfId="201"/>
     <cellStyle name="20% - Accent5" xfId="182" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5 2" xfId="12" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
-    <cellStyle name="20% - Accent5 2 2" xfId="203" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
+    <cellStyle name="20% - Accent5 2" xfId="12"/>
+    <cellStyle name="20% - Accent5 2 2" xfId="203"/>
     <cellStyle name="20% - Accent6" xfId="185" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6 2" xfId="13" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
-    <cellStyle name="20% - Accent6 2 2" xfId="205" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
+    <cellStyle name="20% - Accent6 2" xfId="13"/>
+    <cellStyle name="20% - Accent6 2 2" xfId="205"/>
     <cellStyle name="40% - Accent1" xfId="171" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1 2" xfId="14" xr:uid="{00000000-0005-0000-0000-000013000000}"/>
-    <cellStyle name="40% - Accent1 2 2" xfId="196" xr:uid="{00000000-0005-0000-0000-000014000000}"/>
+    <cellStyle name="40% - Accent1 2" xfId="14"/>
+    <cellStyle name="40% - Accent1 2 2" xfId="196"/>
     <cellStyle name="40% - Accent2" xfId="174" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2 2" xfId="15" xr:uid="{00000000-0005-0000-0000-000016000000}"/>
-    <cellStyle name="40% - Accent2 2 2" xfId="198" xr:uid="{00000000-0005-0000-0000-000017000000}"/>
+    <cellStyle name="40% - Accent2 2" xfId="15"/>
+    <cellStyle name="40% - Accent2 2 2" xfId="198"/>
     <cellStyle name="40% - Accent3" xfId="177" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3 2" xfId="16" xr:uid="{00000000-0005-0000-0000-000019000000}"/>
-    <cellStyle name="40% - Accent3 2 2" xfId="200" xr:uid="{00000000-0005-0000-0000-00001A000000}"/>
+    <cellStyle name="40% - Accent3 2" xfId="16"/>
+    <cellStyle name="40% - Accent3 2 2" xfId="200"/>
     <cellStyle name="40% - Accent4" xfId="180" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4 2" xfId="17" xr:uid="{00000000-0005-0000-0000-00001C000000}"/>
-    <cellStyle name="40% - Accent4 2 2" xfId="202" xr:uid="{00000000-0005-0000-0000-00001D000000}"/>
+    <cellStyle name="40% - Accent4 2" xfId="17"/>
+    <cellStyle name="40% - Accent4 2 2" xfId="202"/>
     <cellStyle name="40% - Accent5" xfId="183" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5 2" xfId="18" xr:uid="{00000000-0005-0000-0000-00001F000000}"/>
-    <cellStyle name="40% - Accent5 2 2" xfId="204" xr:uid="{00000000-0005-0000-0000-000020000000}"/>
+    <cellStyle name="40% - Accent5 2" xfId="18"/>
+    <cellStyle name="40% - Accent5 2 2" xfId="204"/>
     <cellStyle name="40% - Accent6" xfId="186" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6 2" xfId="19" xr:uid="{00000000-0005-0000-0000-000022000000}"/>
-    <cellStyle name="40% - Accent6 2 2" xfId="206" xr:uid="{00000000-0005-0000-0000-000023000000}"/>
-    <cellStyle name="60% - Accent1 2" xfId="20" xr:uid="{00000000-0005-0000-0000-000024000000}"/>
-    <cellStyle name="60% - Accent1 3" xfId="189" xr:uid="{00000000-0005-0000-0000-000025000000}"/>
-    <cellStyle name="60% - Accent2 2" xfId="21" xr:uid="{00000000-0005-0000-0000-000026000000}"/>
-    <cellStyle name="60% - Accent2 3" xfId="190" xr:uid="{00000000-0005-0000-0000-000027000000}"/>
-    <cellStyle name="60% - Accent3 2" xfId="22" xr:uid="{00000000-0005-0000-0000-000028000000}"/>
-    <cellStyle name="60% - Accent3 3" xfId="191" xr:uid="{00000000-0005-0000-0000-000029000000}"/>
-    <cellStyle name="60% - Accent4 2" xfId="23" xr:uid="{00000000-0005-0000-0000-00002A000000}"/>
-    <cellStyle name="60% - Accent4 3" xfId="192" xr:uid="{00000000-0005-0000-0000-00002B000000}"/>
-    <cellStyle name="60% - Accent5 2" xfId="24" xr:uid="{00000000-0005-0000-0000-00002C000000}"/>
-    <cellStyle name="60% - Accent5 3" xfId="193" xr:uid="{00000000-0005-0000-0000-00002D000000}"/>
-    <cellStyle name="60% - Accent6 2" xfId="25" xr:uid="{00000000-0005-0000-0000-00002E000000}"/>
-    <cellStyle name="60% - Accent6 3" xfId="194" xr:uid="{00000000-0005-0000-0000-00002F000000}"/>
+    <cellStyle name="40% - Accent6 2" xfId="19"/>
+    <cellStyle name="40% - Accent6 2 2" xfId="206"/>
+    <cellStyle name="60% - Accent1 2" xfId="20"/>
+    <cellStyle name="60% - Accent1 3" xfId="189"/>
+    <cellStyle name="60% - Accent2 2" xfId="21"/>
+    <cellStyle name="60% - Accent2 3" xfId="190"/>
+    <cellStyle name="60% - Accent3 2" xfId="22"/>
+    <cellStyle name="60% - Accent3 3" xfId="191"/>
+    <cellStyle name="60% - Accent4 2" xfId="23"/>
+    <cellStyle name="60% - Accent4 3" xfId="192"/>
+    <cellStyle name="60% - Accent5 2" xfId="24"/>
+    <cellStyle name="60% - Accent5 3" xfId="193"/>
+    <cellStyle name="60% - Accent6 2" xfId="25"/>
+    <cellStyle name="60% - Accent6 3" xfId="194"/>
     <cellStyle name="Accent1" xfId="169" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent1 2" xfId="26" xr:uid="{00000000-0005-0000-0000-000031000000}"/>
+    <cellStyle name="Accent1 2" xfId="26"/>
     <cellStyle name="Accent2" xfId="172" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent2 2" xfId="27" xr:uid="{00000000-0005-0000-0000-000033000000}"/>
+    <cellStyle name="Accent2 2" xfId="27"/>
     <cellStyle name="Accent3" xfId="175" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent3 2" xfId="28" xr:uid="{00000000-0005-0000-0000-000035000000}"/>
+    <cellStyle name="Accent3 2" xfId="28"/>
     <cellStyle name="Accent4" xfId="178" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent4 2" xfId="29" xr:uid="{00000000-0005-0000-0000-000037000000}"/>
+    <cellStyle name="Accent4 2" xfId="29"/>
     <cellStyle name="Accent5" xfId="181" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent5 2" xfId="30" xr:uid="{00000000-0005-0000-0000-000039000000}"/>
+    <cellStyle name="Accent5 2" xfId="30"/>
     <cellStyle name="Accent6" xfId="184" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Accent6 2" xfId="31" xr:uid="{00000000-0005-0000-0000-00003B000000}"/>
+    <cellStyle name="Accent6 2" xfId="31"/>
     <cellStyle name="Bad" xfId="159" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Bad 2" xfId="32" xr:uid="{00000000-0005-0000-0000-00003D000000}"/>
-    <cellStyle name="Body: normal cell" xfId="4" xr:uid="{00000000-0005-0000-0000-00003E000000}"/>
-    <cellStyle name="Body: normal cell 2" xfId="33" xr:uid="{00000000-0005-0000-0000-00003F000000}"/>
+    <cellStyle name="Bad 2" xfId="32"/>
+    <cellStyle name="Body: normal cell" xfId="4"/>
+    <cellStyle name="Body: normal cell 2" xfId="33"/>
     <cellStyle name="Calculation" xfId="162" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Calculation 2" xfId="34" xr:uid="{00000000-0005-0000-0000-000041000000}"/>
+    <cellStyle name="Calculation 2" xfId="34"/>
     <cellStyle name="Check Cell" xfId="164" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Check Cell 2" xfId="35" xr:uid="{00000000-0005-0000-0000-000043000000}"/>
-    <cellStyle name="Column heading" xfId="36" xr:uid="{00000000-0005-0000-0000-000044000000}"/>
-    <cellStyle name="Comma 2" xfId="37" xr:uid="{00000000-0005-0000-0000-000045000000}"/>
-    <cellStyle name="Comma 2 2" xfId="38" xr:uid="{00000000-0005-0000-0000-000046000000}"/>
-    <cellStyle name="Comma 3" xfId="39" xr:uid="{00000000-0005-0000-0000-000047000000}"/>
-    <cellStyle name="Comma 4" xfId="40" xr:uid="{00000000-0005-0000-0000-000048000000}"/>
-    <cellStyle name="Comma 5" xfId="41" xr:uid="{00000000-0005-0000-0000-000049000000}"/>
-    <cellStyle name="Comma 6" xfId="42" xr:uid="{00000000-0005-0000-0000-00004A000000}"/>
-    <cellStyle name="Comma 7" xfId="43" xr:uid="{00000000-0005-0000-0000-00004B000000}"/>
-    <cellStyle name="Comma 8" xfId="44" xr:uid="{00000000-0005-0000-0000-00004C000000}"/>
-    <cellStyle name="Corner heading" xfId="45" xr:uid="{00000000-0005-0000-0000-00004D000000}"/>
-    <cellStyle name="Currency 2" xfId="46" xr:uid="{00000000-0005-0000-0000-00004E000000}"/>
-    <cellStyle name="Currency 3" xfId="47" xr:uid="{00000000-0005-0000-0000-00004F000000}"/>
-    <cellStyle name="Currency 3 2" xfId="48" xr:uid="{00000000-0005-0000-0000-000050000000}"/>
-    <cellStyle name="Data" xfId="49" xr:uid="{00000000-0005-0000-0000-000051000000}"/>
-    <cellStyle name="Data 2" xfId="50" xr:uid="{00000000-0005-0000-0000-000052000000}"/>
-    <cellStyle name="Data no deci" xfId="51" xr:uid="{00000000-0005-0000-0000-000053000000}"/>
-    <cellStyle name="Data Superscript" xfId="52" xr:uid="{00000000-0005-0000-0000-000054000000}"/>
-    <cellStyle name="Data_1-1A-Regular" xfId="53" xr:uid="{00000000-0005-0000-0000-000055000000}"/>
+    <cellStyle name="Check Cell 2" xfId="35"/>
+    <cellStyle name="Column heading" xfId="36"/>
+    <cellStyle name="Comma 2" xfId="37"/>
+    <cellStyle name="Comma 2 2" xfId="38"/>
+    <cellStyle name="Comma 3" xfId="39"/>
+    <cellStyle name="Comma 4" xfId="40"/>
+    <cellStyle name="Comma 5" xfId="41"/>
+    <cellStyle name="Comma 6" xfId="42"/>
+    <cellStyle name="Comma 7" xfId="43"/>
+    <cellStyle name="Comma 8" xfId="44"/>
+    <cellStyle name="Corner heading" xfId="45"/>
+    <cellStyle name="Currency 2" xfId="46"/>
+    <cellStyle name="Currency 3" xfId="47"/>
+    <cellStyle name="Currency 3 2" xfId="48"/>
+    <cellStyle name="Data" xfId="49"/>
+    <cellStyle name="Data 2" xfId="50"/>
+    <cellStyle name="Data no deci" xfId="51"/>
+    <cellStyle name="Data Superscript" xfId="52"/>
+    <cellStyle name="Data_1-1A-Regular" xfId="53"/>
     <cellStyle name="Explanatory Text" xfId="167" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text 2" xfId="54" xr:uid="{00000000-0005-0000-0000-000057000000}"/>
-    <cellStyle name="Font: Calibri, 9pt regular" xfId="6" xr:uid="{00000000-0005-0000-0000-000058000000}"/>
-    <cellStyle name="Font: Calibri, 9pt regular 2" xfId="55" xr:uid="{00000000-0005-0000-0000-000059000000}"/>
-    <cellStyle name="Footnotes: top row" xfId="2" xr:uid="{00000000-0005-0000-0000-00005A000000}"/>
-    <cellStyle name="Footnotes: top row 2" xfId="56" xr:uid="{00000000-0005-0000-0000-00005B000000}"/>
+    <cellStyle name="Explanatory Text 2" xfId="54"/>
+    <cellStyle name="Font: Calibri, 9pt regular" xfId="6"/>
+    <cellStyle name="Font: Calibri, 9pt regular 2" xfId="55"/>
+    <cellStyle name="Footnotes: top row" xfId="2"/>
+    <cellStyle name="Footnotes: top row 2" xfId="56"/>
     <cellStyle name="Good" xfId="158" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Good 2" xfId="57" xr:uid="{00000000-0005-0000-0000-00005D000000}"/>
-    <cellStyle name="Header: bottom row" xfId="5" xr:uid="{00000000-0005-0000-0000-00005E000000}"/>
-    <cellStyle name="Header: bottom row 2" xfId="58" xr:uid="{00000000-0005-0000-0000-00005F000000}"/>
+    <cellStyle name="Good 2" xfId="57"/>
+    <cellStyle name="Header: bottom row" xfId="5"/>
+    <cellStyle name="Header: bottom row 2" xfId="58"/>
     <cellStyle name="Heading 1" xfId="154" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 1 2" xfId="59" xr:uid="{00000000-0005-0000-0000-000061000000}"/>
+    <cellStyle name="Heading 1 2" xfId="59"/>
     <cellStyle name="Heading 2" xfId="155" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 2 2" xfId="60" xr:uid="{00000000-0005-0000-0000-000063000000}"/>
+    <cellStyle name="Heading 2 2" xfId="60"/>
     <cellStyle name="Heading 3" xfId="156" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 3 2" xfId="61" xr:uid="{00000000-0005-0000-0000-000065000000}"/>
+    <cellStyle name="Heading 3 2" xfId="61"/>
     <cellStyle name="Heading 4" xfId="157" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Heading 4 2" xfId="62" xr:uid="{00000000-0005-0000-0000-000067000000}"/>
-    <cellStyle name="Hed Side" xfId="63" xr:uid="{00000000-0005-0000-0000-000068000000}"/>
-    <cellStyle name="Hed Side 2" xfId="64" xr:uid="{00000000-0005-0000-0000-000069000000}"/>
-    <cellStyle name="Hed Side bold" xfId="65" xr:uid="{00000000-0005-0000-0000-00006A000000}"/>
-    <cellStyle name="Hed Side Indent" xfId="66" xr:uid="{00000000-0005-0000-0000-00006B000000}"/>
-    <cellStyle name="Hed Side Regular" xfId="67" xr:uid="{00000000-0005-0000-0000-00006C000000}"/>
-    <cellStyle name="Hed Side_1-1A-Regular" xfId="68" xr:uid="{00000000-0005-0000-0000-00006D000000}"/>
-    <cellStyle name="Hed Top" xfId="69" xr:uid="{00000000-0005-0000-0000-00006E000000}"/>
-    <cellStyle name="Hed Top - SECTION" xfId="70" xr:uid="{00000000-0005-0000-0000-00006F000000}"/>
-    <cellStyle name="Hed Top_3-new4" xfId="71" xr:uid="{00000000-0005-0000-0000-000070000000}"/>
+    <cellStyle name="Heading 4 2" xfId="62"/>
+    <cellStyle name="Hed Side" xfId="63"/>
+    <cellStyle name="Hed Side 2" xfId="64"/>
+    <cellStyle name="Hed Side bold" xfId="65"/>
+    <cellStyle name="Hed Side Indent" xfId="66"/>
+    <cellStyle name="Hed Side Regular" xfId="67"/>
+    <cellStyle name="Hed Side_1-1A-Regular" xfId="68"/>
+    <cellStyle name="Hed Top" xfId="69"/>
+    <cellStyle name="Hed Top - SECTION" xfId="70"/>
+    <cellStyle name="Hed Top_3-new4" xfId="71"/>
     <cellStyle name="Hyperlink" xfId="187" builtinId="8"/>
-    <cellStyle name="Hyperlink 2" xfId="72" xr:uid="{00000000-0005-0000-0000-000072000000}"/>
+    <cellStyle name="Hyperlink 2" xfId="72"/>
     <cellStyle name="Input" xfId="160" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Input 2" xfId="73" xr:uid="{00000000-0005-0000-0000-000074000000}"/>
+    <cellStyle name="Input 2" xfId="73"/>
     <cellStyle name="Linked Cell" xfId="163" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Linked Cell 2" xfId="74" xr:uid="{00000000-0005-0000-0000-000076000000}"/>
-    <cellStyle name="Neutral 2" xfId="75" xr:uid="{00000000-0005-0000-0000-000077000000}"/>
-    <cellStyle name="Neutral 3" xfId="188" xr:uid="{00000000-0005-0000-0000-000078000000}"/>
+    <cellStyle name="Linked Cell 2" xfId="74"/>
+    <cellStyle name="Neutral 2" xfId="75"/>
+    <cellStyle name="Neutral 3" xfId="188"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 10" xfId="76" xr:uid="{00000000-0005-0000-0000-00007A000000}"/>
-    <cellStyle name="Normal 11" xfId="77" xr:uid="{00000000-0005-0000-0000-00007B000000}"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-00007C000000}"/>
-    <cellStyle name="Normal 2 2" xfId="78" xr:uid="{00000000-0005-0000-0000-00007D000000}"/>
-    <cellStyle name="Normal 2 3" xfId="79" xr:uid="{00000000-0005-0000-0000-00007E000000}"/>
-    <cellStyle name="Normal 3" xfId="80" xr:uid="{00000000-0005-0000-0000-00007F000000}"/>
-    <cellStyle name="Normal 3 2" xfId="81" xr:uid="{00000000-0005-0000-0000-000080000000}"/>
-    <cellStyle name="Normal 3 2 2" xfId="82" xr:uid="{00000000-0005-0000-0000-000081000000}"/>
-    <cellStyle name="Normal 3 2 2 2" xfId="83" xr:uid="{00000000-0005-0000-0000-000082000000}"/>
-    <cellStyle name="Normal 3 2 3" xfId="84" xr:uid="{00000000-0005-0000-0000-000083000000}"/>
-    <cellStyle name="Normal 3 3" xfId="85" xr:uid="{00000000-0005-0000-0000-000084000000}"/>
-    <cellStyle name="Normal 3 3 2" xfId="86" xr:uid="{00000000-0005-0000-0000-000085000000}"/>
-    <cellStyle name="Normal 3 3 2 2" xfId="87" xr:uid="{00000000-0005-0000-0000-000086000000}"/>
-    <cellStyle name="Normal 3 3 3" xfId="88" xr:uid="{00000000-0005-0000-0000-000087000000}"/>
-    <cellStyle name="Normal 3 4" xfId="89" xr:uid="{00000000-0005-0000-0000-000088000000}"/>
-    <cellStyle name="Normal 3 4 2" xfId="90" xr:uid="{00000000-0005-0000-0000-000089000000}"/>
-    <cellStyle name="Normal 3 5" xfId="91" xr:uid="{00000000-0005-0000-0000-00008A000000}"/>
-    <cellStyle name="Normal 3 6" xfId="92" xr:uid="{00000000-0005-0000-0000-00008B000000}"/>
-    <cellStyle name="Normal 3 7" xfId="93" xr:uid="{00000000-0005-0000-0000-00008C000000}"/>
-    <cellStyle name="Normal 4" xfId="94" xr:uid="{00000000-0005-0000-0000-00008D000000}"/>
-    <cellStyle name="Normal 4 2" xfId="95" xr:uid="{00000000-0005-0000-0000-00008E000000}"/>
-    <cellStyle name="Normal 4 2 2" xfId="96" xr:uid="{00000000-0005-0000-0000-00008F000000}"/>
-    <cellStyle name="Normal 4 2 2 2" xfId="97" xr:uid="{00000000-0005-0000-0000-000090000000}"/>
-    <cellStyle name="Normal 4 2 3" xfId="98" xr:uid="{00000000-0005-0000-0000-000091000000}"/>
-    <cellStyle name="Normal 4 3" xfId="99" xr:uid="{00000000-0005-0000-0000-000092000000}"/>
-    <cellStyle name="Normal 4 3 2" xfId="100" xr:uid="{00000000-0005-0000-0000-000093000000}"/>
-    <cellStyle name="Normal 4 3 2 2" xfId="101" xr:uid="{00000000-0005-0000-0000-000094000000}"/>
-    <cellStyle name="Normal 4 3 3" xfId="102" xr:uid="{00000000-0005-0000-0000-000095000000}"/>
-    <cellStyle name="Normal 4 4" xfId="103" xr:uid="{00000000-0005-0000-0000-000096000000}"/>
-    <cellStyle name="Normal 4 4 2" xfId="104" xr:uid="{00000000-0005-0000-0000-000097000000}"/>
-    <cellStyle name="Normal 4 5" xfId="105" xr:uid="{00000000-0005-0000-0000-000098000000}"/>
-    <cellStyle name="Normal 4 6" xfId="106" xr:uid="{00000000-0005-0000-0000-000099000000}"/>
-    <cellStyle name="Normal 4 7" xfId="107" xr:uid="{00000000-0005-0000-0000-00009A000000}"/>
-    <cellStyle name="Normal 5" xfId="108" xr:uid="{00000000-0005-0000-0000-00009B000000}"/>
-    <cellStyle name="Normal 5 2" xfId="109" xr:uid="{00000000-0005-0000-0000-00009C000000}"/>
-    <cellStyle name="Normal 5 3" xfId="110" xr:uid="{00000000-0005-0000-0000-00009D000000}"/>
-    <cellStyle name="Normal 6" xfId="111" xr:uid="{00000000-0005-0000-0000-00009E000000}"/>
-    <cellStyle name="Normal 6 2" xfId="112" xr:uid="{00000000-0005-0000-0000-00009F000000}"/>
-    <cellStyle name="Normal 7" xfId="113" xr:uid="{00000000-0005-0000-0000-0000A0000000}"/>
-    <cellStyle name="Normal 7 2" xfId="114" xr:uid="{00000000-0005-0000-0000-0000A1000000}"/>
-    <cellStyle name="Normal 8" xfId="115" xr:uid="{00000000-0005-0000-0000-0000A2000000}"/>
-    <cellStyle name="Normal 9" xfId="116" xr:uid="{00000000-0005-0000-0000-0000A3000000}"/>
+    <cellStyle name="Normal 10" xfId="76"/>
+    <cellStyle name="Normal 11" xfId="77"/>
+    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2 2" xfId="78"/>
+    <cellStyle name="Normal 2 3" xfId="79"/>
+    <cellStyle name="Normal 3" xfId="80"/>
+    <cellStyle name="Normal 3 2" xfId="81"/>
+    <cellStyle name="Normal 3 2 2" xfId="82"/>
+    <cellStyle name="Normal 3 2 2 2" xfId="83"/>
+    <cellStyle name="Normal 3 2 3" xfId="84"/>
+    <cellStyle name="Normal 3 3" xfId="85"/>
+    <cellStyle name="Normal 3 3 2" xfId="86"/>
+    <cellStyle name="Normal 3 3 2 2" xfId="87"/>
+    <cellStyle name="Normal 3 3 3" xfId="88"/>
+    <cellStyle name="Normal 3 4" xfId="89"/>
+    <cellStyle name="Normal 3 4 2" xfId="90"/>
+    <cellStyle name="Normal 3 5" xfId="91"/>
+    <cellStyle name="Normal 3 6" xfId="92"/>
+    <cellStyle name="Normal 3 7" xfId="93"/>
+    <cellStyle name="Normal 4" xfId="94"/>
+    <cellStyle name="Normal 4 2" xfId="95"/>
+    <cellStyle name="Normal 4 2 2" xfId="96"/>
+    <cellStyle name="Normal 4 2 2 2" xfId="97"/>
+    <cellStyle name="Normal 4 2 3" xfId="98"/>
+    <cellStyle name="Normal 4 3" xfId="99"/>
+    <cellStyle name="Normal 4 3 2" xfId="100"/>
+    <cellStyle name="Normal 4 3 2 2" xfId="101"/>
+    <cellStyle name="Normal 4 3 3" xfId="102"/>
+    <cellStyle name="Normal 4 4" xfId="103"/>
+    <cellStyle name="Normal 4 4 2" xfId="104"/>
+    <cellStyle name="Normal 4 5" xfId="105"/>
+    <cellStyle name="Normal 4 6" xfId="106"/>
+    <cellStyle name="Normal 4 7" xfId="107"/>
+    <cellStyle name="Normal 5" xfId="108"/>
+    <cellStyle name="Normal 5 2" xfId="109"/>
+    <cellStyle name="Normal 5 3" xfId="110"/>
+    <cellStyle name="Normal 6" xfId="111"/>
+    <cellStyle name="Normal 6 2" xfId="112"/>
+    <cellStyle name="Normal 7" xfId="113"/>
+    <cellStyle name="Normal 7 2" xfId="114"/>
+    <cellStyle name="Normal 8" xfId="115"/>
+    <cellStyle name="Normal 9" xfId="116"/>
     <cellStyle name="Note" xfId="166" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Note 2" xfId="117" xr:uid="{00000000-0005-0000-0000-0000A5000000}"/>
-    <cellStyle name="Note 2 2" xfId="118" xr:uid="{00000000-0005-0000-0000-0000A6000000}"/>
+    <cellStyle name="Note 2" xfId="117"/>
+    <cellStyle name="Note 2 2" xfId="118"/>
     <cellStyle name="Output" xfId="161" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Output 2" xfId="119" xr:uid="{00000000-0005-0000-0000-0000A8000000}"/>
-    <cellStyle name="Parent row" xfId="3" xr:uid="{00000000-0005-0000-0000-0000A9000000}"/>
-    <cellStyle name="Parent row 2" xfId="120" xr:uid="{00000000-0005-0000-0000-0000AA000000}"/>
-    <cellStyle name="Percent 2" xfId="121" xr:uid="{00000000-0005-0000-0000-0000AB000000}"/>
-    <cellStyle name="Percent 2 2" xfId="122" xr:uid="{00000000-0005-0000-0000-0000AC000000}"/>
-    <cellStyle name="Percent 3" xfId="123" xr:uid="{00000000-0005-0000-0000-0000AD000000}"/>
-    <cellStyle name="Percent 3 2" xfId="124" xr:uid="{00000000-0005-0000-0000-0000AE000000}"/>
-    <cellStyle name="Percent 4" xfId="125" xr:uid="{00000000-0005-0000-0000-0000AF000000}"/>
-    <cellStyle name="Reference" xfId="126" xr:uid="{00000000-0005-0000-0000-0000B0000000}"/>
-    <cellStyle name="Row heading" xfId="127" xr:uid="{00000000-0005-0000-0000-0000B1000000}"/>
-    <cellStyle name="Source Hed" xfId="128" xr:uid="{00000000-0005-0000-0000-0000B2000000}"/>
-    <cellStyle name="Source Letter" xfId="129" xr:uid="{00000000-0005-0000-0000-0000B3000000}"/>
-    <cellStyle name="Source Superscript" xfId="130" xr:uid="{00000000-0005-0000-0000-0000B4000000}"/>
-    <cellStyle name="Source Superscript 2" xfId="131" xr:uid="{00000000-0005-0000-0000-0000B5000000}"/>
-    <cellStyle name="Source Text" xfId="132" xr:uid="{00000000-0005-0000-0000-0000B6000000}"/>
-    <cellStyle name="Source Text 2" xfId="133" xr:uid="{00000000-0005-0000-0000-0000B7000000}"/>
-    <cellStyle name="State" xfId="134" xr:uid="{00000000-0005-0000-0000-0000B8000000}"/>
-    <cellStyle name="Superscript" xfId="135" xr:uid="{00000000-0005-0000-0000-0000B9000000}"/>
-    <cellStyle name="Table Data" xfId="136" xr:uid="{00000000-0005-0000-0000-0000BA000000}"/>
-    <cellStyle name="Table Head Top" xfId="137" xr:uid="{00000000-0005-0000-0000-0000BB000000}"/>
-    <cellStyle name="Table Hed Side" xfId="138" xr:uid="{00000000-0005-0000-0000-0000BC000000}"/>
-    <cellStyle name="Table title" xfId="7" xr:uid="{00000000-0005-0000-0000-0000BD000000}"/>
-    <cellStyle name="Table title 2" xfId="139" xr:uid="{00000000-0005-0000-0000-0000BE000000}"/>
+    <cellStyle name="Output 2" xfId="119"/>
+    <cellStyle name="Parent row" xfId="3"/>
+    <cellStyle name="Parent row 2" xfId="120"/>
+    <cellStyle name="Percent 2" xfId="121"/>
+    <cellStyle name="Percent 2 2" xfId="122"/>
+    <cellStyle name="Percent 3" xfId="123"/>
+    <cellStyle name="Percent 3 2" xfId="124"/>
+    <cellStyle name="Percent 4" xfId="125"/>
+    <cellStyle name="Reference" xfId="126"/>
+    <cellStyle name="Row heading" xfId="127"/>
+    <cellStyle name="Source Hed" xfId="128"/>
+    <cellStyle name="Source Letter" xfId="129"/>
+    <cellStyle name="Source Superscript" xfId="130"/>
+    <cellStyle name="Source Superscript 2" xfId="131"/>
+    <cellStyle name="Source Text" xfId="132"/>
+    <cellStyle name="Source Text 2" xfId="133"/>
+    <cellStyle name="State" xfId="134"/>
+    <cellStyle name="Superscript" xfId="135"/>
+    <cellStyle name="Table Data" xfId="136"/>
+    <cellStyle name="Table Head Top" xfId="137"/>
+    <cellStyle name="Table Hed Side" xfId="138"/>
+    <cellStyle name="Table title" xfId="7"/>
+    <cellStyle name="Table title 2" xfId="139"/>
     <cellStyle name="Title" xfId="153" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Title 2" xfId="140" xr:uid="{00000000-0005-0000-0000-0000C0000000}"/>
-    <cellStyle name="Title Text" xfId="141" xr:uid="{00000000-0005-0000-0000-0000C1000000}"/>
-    <cellStyle name="Title Text 1" xfId="142" xr:uid="{00000000-0005-0000-0000-0000C2000000}"/>
-    <cellStyle name="Title Text 2" xfId="143" xr:uid="{00000000-0005-0000-0000-0000C3000000}"/>
-    <cellStyle name="Title-1" xfId="144" xr:uid="{00000000-0005-0000-0000-0000C4000000}"/>
-    <cellStyle name="Title-2" xfId="145" xr:uid="{00000000-0005-0000-0000-0000C5000000}"/>
-    <cellStyle name="Title-3" xfId="146" xr:uid="{00000000-0005-0000-0000-0000C6000000}"/>
+    <cellStyle name="Title 2" xfId="140"/>
+    <cellStyle name="Title Text" xfId="141"/>
+    <cellStyle name="Title Text 1" xfId="142"/>
+    <cellStyle name="Title Text 2" xfId="143"/>
+    <cellStyle name="Title-1" xfId="144"/>
+    <cellStyle name="Title-2" xfId="145"/>
+    <cellStyle name="Title-3" xfId="146"/>
     <cellStyle name="Total" xfId="168" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Total 2" xfId="147" xr:uid="{00000000-0005-0000-0000-0000C8000000}"/>
+    <cellStyle name="Total 2" xfId="147"/>
     <cellStyle name="Warning Text" xfId="165" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="Warning Text 2" xfId="148" xr:uid="{00000000-0005-0000-0000-0000CA000000}"/>
-    <cellStyle name="Wrap" xfId="149" xr:uid="{00000000-0005-0000-0000-0000CB000000}"/>
-    <cellStyle name="Wrap Bold" xfId="150" xr:uid="{00000000-0005-0000-0000-0000CC000000}"/>
-    <cellStyle name="Wrap Title" xfId="151" xr:uid="{00000000-0005-0000-0000-0000CD000000}"/>
-    <cellStyle name="Wrap_NTS99-~11" xfId="152" xr:uid="{00000000-0005-0000-0000-0000CE000000}"/>
+    <cellStyle name="Warning Text 2" xfId="148"/>
+    <cellStyle name="Wrap" xfId="149"/>
+    <cellStyle name="Wrap Bold" xfId="150"/>
+    <cellStyle name="Wrap Title" xfId="151"/>
+    <cellStyle name="Wrap_NTS99-~11" xfId="152"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -3666,23 +3664,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -3718,23 +3699,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -3910,7 +3874,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -4020,7 +3984,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B7" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B7" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -4028,7 +3992,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AK107"/>
   <sheetViews>
     <sheetView topLeftCell="M1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
@@ -10712,44 +10676,44 @@
     </row>
     <row r="86" spans="1:37" ht="15" customHeight="1" thickBot="1"/>
     <row r="87" spans="1:37" ht="15" customHeight="1">
-      <c r="B87" s="99" t="s">
+      <c r="B87" s="100" t="s">
         <v>7</v>
       </c>
-      <c r="C87" s="99"/>
-      <c r="D87" s="99"/>
-      <c r="E87" s="99"/>
-      <c r="F87" s="99"/>
-      <c r="G87" s="99"/>
-      <c r="H87" s="99"/>
-      <c r="I87" s="99"/>
-      <c r="J87" s="99"/>
-      <c r="K87" s="99"/>
-      <c r="L87" s="99"/>
-      <c r="M87" s="99"/>
-      <c r="N87" s="99"/>
-      <c r="O87" s="99"/>
-      <c r="P87" s="99"/>
-      <c r="Q87" s="99"/>
-      <c r="R87" s="99"/>
-      <c r="S87" s="99"/>
-      <c r="T87" s="99"/>
-      <c r="U87" s="99"/>
-      <c r="V87" s="99"/>
-      <c r="W87" s="99"/>
-      <c r="X87" s="99"/>
-      <c r="Y87" s="99"/>
-      <c r="Z87" s="99"/>
-      <c r="AA87" s="99"/>
-      <c r="AB87" s="99"/>
-      <c r="AC87" s="99"/>
-      <c r="AD87" s="99"/>
-      <c r="AE87" s="99"/>
-      <c r="AF87" s="99"/>
-      <c r="AG87" s="99"/>
-      <c r="AH87" s="99"/>
-      <c r="AI87" s="99"/>
-      <c r="AJ87" s="99"/>
-      <c r="AK87" s="99"/>
+      <c r="C87" s="100"/>
+      <c r="D87" s="100"/>
+      <c r="E87" s="100"/>
+      <c r="F87" s="100"/>
+      <c r="G87" s="100"/>
+      <c r="H87" s="100"/>
+      <c r="I87" s="100"/>
+      <c r="J87" s="100"/>
+      <c r="K87" s="100"/>
+      <c r="L87" s="100"/>
+      <c r="M87" s="100"/>
+      <c r="N87" s="100"/>
+      <c r="O87" s="100"/>
+      <c r="P87" s="100"/>
+      <c r="Q87" s="100"/>
+      <c r="R87" s="100"/>
+      <c r="S87" s="100"/>
+      <c r="T87" s="100"/>
+      <c r="U87" s="100"/>
+      <c r="V87" s="100"/>
+      <c r="W87" s="100"/>
+      <c r="X87" s="100"/>
+      <c r="Y87" s="100"/>
+      <c r="Z87" s="100"/>
+      <c r="AA87" s="100"/>
+      <c r="AB87" s="100"/>
+      <c r="AC87" s="100"/>
+      <c r="AD87" s="100"/>
+      <c r="AE87" s="100"/>
+      <c r="AF87" s="100"/>
+      <c r="AG87" s="100"/>
+      <c r="AH87" s="100"/>
+      <c r="AI87" s="100"/>
+      <c r="AJ87" s="100"/>
+      <c r="AK87" s="100"/>
     </row>
     <row r="88" spans="1:37" ht="15" customHeight="1">
       <c r="B88" s="15" t="s">
@@ -10860,7 +10824,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6028C1B8-C9CE-49D0-991F-03EFC0A5C7EF}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL91"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
@@ -17679,45 +17643,45 @@
     </row>
     <row r="76" spans="1:38">
       <c r="A76" s="85"/>
-      <c r="B76" s="99" t="s">
+      <c r="B76" s="100" t="s">
         <v>446</v>
       </c>
-      <c r="C76" s="99"/>
-      <c r="D76" s="99"/>
-      <c r="E76" s="99"/>
-      <c r="F76" s="99"/>
-      <c r="G76" s="99"/>
-      <c r="H76" s="99"/>
-      <c r="I76" s="99"/>
-      <c r="J76" s="99"/>
-      <c r="K76" s="99"/>
-      <c r="L76" s="99"/>
-      <c r="M76" s="99"/>
-      <c r="N76" s="99"/>
-      <c r="O76" s="99"/>
-      <c r="P76" s="99"/>
-      <c r="Q76" s="99"/>
-      <c r="R76" s="99"/>
-      <c r="S76" s="99"/>
-      <c r="T76" s="99"/>
-      <c r="U76" s="99"/>
-      <c r="V76" s="99"/>
-      <c r="W76" s="99"/>
-      <c r="X76" s="99"/>
-      <c r="Y76" s="99"/>
-      <c r="Z76" s="99"/>
-      <c r="AA76" s="99"/>
-      <c r="AB76" s="99"/>
-      <c r="AC76" s="99"/>
-      <c r="AD76" s="99"/>
-      <c r="AE76" s="99"/>
-      <c r="AF76" s="99"/>
-      <c r="AG76" s="99"/>
-      <c r="AH76" s="99"/>
-      <c r="AI76" s="99"/>
-      <c r="AJ76" s="99"/>
-      <c r="AK76" s="99"/>
-      <c r="AL76" s="99"/>
+      <c r="C76" s="100"/>
+      <c r="D76" s="100"/>
+      <c r="E76" s="100"/>
+      <c r="F76" s="100"/>
+      <c r="G76" s="100"/>
+      <c r="H76" s="100"/>
+      <c r="I76" s="100"/>
+      <c r="J76" s="100"/>
+      <c r="K76" s="100"/>
+      <c r="L76" s="100"/>
+      <c r="M76" s="100"/>
+      <c r="N76" s="100"/>
+      <c r="O76" s="100"/>
+      <c r="P76" s="100"/>
+      <c r="Q76" s="100"/>
+      <c r="R76" s="100"/>
+      <c r="S76" s="100"/>
+      <c r="T76" s="100"/>
+      <c r="U76" s="100"/>
+      <c r="V76" s="100"/>
+      <c r="W76" s="100"/>
+      <c r="X76" s="100"/>
+      <c r="Y76" s="100"/>
+      <c r="Z76" s="100"/>
+      <c r="AA76" s="100"/>
+      <c r="AB76" s="100"/>
+      <c r="AC76" s="100"/>
+      <c r="AD76" s="100"/>
+      <c r="AE76" s="100"/>
+      <c r="AF76" s="100"/>
+      <c r="AG76" s="100"/>
+      <c r="AH76" s="100"/>
+      <c r="AI76" s="100"/>
+      <c r="AJ76" s="100"/>
+      <c r="AK76" s="100"/>
+      <c r="AL76" s="100"/>
     </row>
     <row r="77" spans="1:38">
       <c r="A77" s="85"/>
@@ -17951,7 +17915,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AK214"/>
   <sheetViews>
     <sheetView topLeftCell="B49" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
@@ -23490,106 +23454,106 @@
       <c r="B74" s="77" t="s">
         <v>152</v>
       </c>
-      <c r="C74" s="100">
+      <c r="C74" s="99">
         <v>34.316971000000002</v>
       </c>
-      <c r="D74" s="100">
+      <c r="D74" s="99">
         <v>34.648293000000002</v>
       </c>
-      <c r="E74" s="100">
+      <c r="E74" s="99">
         <v>35.024445</v>
       </c>
-      <c r="F74" s="100">
+      <c r="F74" s="99">
         <v>35.440758000000002</v>
       </c>
-      <c r="G74" s="100">
+      <c r="G74" s="99">
         <v>35.108142999999998</v>
       </c>
-      <c r="H74" s="100">
+      <c r="H74" s="99">
         <v>35.142937000000003</v>
       </c>
-      <c r="I74" s="100">
+      <c r="I74" s="99">
         <v>35.519855</v>
       </c>
-      <c r="J74" s="100">
+      <c r="J74" s="99">
         <v>35.833542000000001</v>
       </c>
-      <c r="K74" s="100">
+      <c r="K74" s="99">
         <v>36.087555000000002</v>
       </c>
-      <c r="L74" s="100">
+      <c r="L74" s="99">
         <v>36.130946999999999</v>
       </c>
-      <c r="M74" s="100">
+      <c r="M74" s="99">
         <v>36.074615000000001</v>
       </c>
-      <c r="N74" s="100">
+      <c r="N74" s="99">
         <v>36.169688999999998</v>
       </c>
-      <c r="O74" s="100">
+      <c r="O74" s="99">
         <v>36.276919999999997</v>
       </c>
-      <c r="P74" s="100">
+      <c r="P74" s="99">
         <v>36.561461999999999</v>
       </c>
-      <c r="Q74" s="100">
+      <c r="Q74" s="99">
         <v>36.822121000000003</v>
       </c>
-      <c r="R74" s="100">
+      <c r="R74" s="99">
         <v>37.041415999999998</v>
       </c>
-      <c r="S74" s="100">
+      <c r="S74" s="99">
         <v>37.319930999999997</v>
       </c>
-      <c r="T74" s="100">
+      <c r="T74" s="99">
         <v>37.567036000000002</v>
       </c>
-      <c r="U74" s="100">
+      <c r="U74" s="99">
         <v>37.770184</v>
       </c>
-      <c r="V74" s="100">
+      <c r="V74" s="99">
         <v>37.998874999999998</v>
       </c>
-      <c r="W74" s="100">
+      <c r="W74" s="99">
         <v>38.243271</v>
       </c>
-      <c r="X74" s="100">
+      <c r="X74" s="99">
         <v>38.461266000000002</v>
       </c>
-      <c r="Y74" s="100">
+      <c r="Y74" s="99">
         <v>38.641711999999998</v>
       </c>
-      <c r="Z74" s="100">
+      <c r="Z74" s="99">
         <v>38.852454999999999</v>
       </c>
-      <c r="AA74" s="100">
+      <c r="AA74" s="99">
         <v>39.014774000000003</v>
       </c>
-      <c r="AB74" s="100">
+      <c r="AB74" s="99">
         <v>38.972732999999998</v>
       </c>
-      <c r="AC74" s="100">
+      <c r="AC74" s="99">
         <v>39.251961000000001</v>
       </c>
-      <c r="AD74" s="100">
+      <c r="AD74" s="99">
         <v>39.240775999999997</v>
       </c>
-      <c r="AE74" s="100">
+      <c r="AE74" s="99">
         <v>39.480815999999997</v>
       </c>
-      <c r="AF74" s="100">
+      <c r="AF74" s="99">
         <v>39.394114999999999</v>
       </c>
-      <c r="AG74" s="100">
+      <c r="AG74" s="99">
         <v>39.419665999999999</v>
       </c>
-      <c r="AH74" s="100">
+      <c r="AH74" s="99">
         <v>39.433632000000003</v>
       </c>
-      <c r="AI74" s="100">
+      <c r="AI74" s="99">
         <v>39.397224000000001</v>
       </c>
-      <c r="AJ74" s="100">
+      <c r="AJ74" s="99">
         <v>39.362923000000002</v>
       </c>
       <c r="AK74" s="79">
@@ -36746,44 +36710,44 @@
     </row>
     <row r="204" spans="1:37" ht="15" customHeight="1" thickBot="1"/>
     <row r="205" spans="1:37" ht="15" customHeight="1">
-      <c r="B205" s="99" t="s">
+      <c r="B205" s="100" t="s">
         <v>388</v>
       </c>
-      <c r="C205" s="99"/>
-      <c r="D205" s="99"/>
-      <c r="E205" s="99"/>
-      <c r="F205" s="99"/>
-      <c r="G205" s="99"/>
-      <c r="H205" s="99"/>
-      <c r="I205" s="99"/>
-      <c r="J205" s="99"/>
-      <c r="K205" s="99"/>
-      <c r="L205" s="99"/>
-      <c r="M205" s="99"/>
-      <c r="N205" s="99"/>
-      <c r="O205" s="99"/>
-      <c r="P205" s="99"/>
-      <c r="Q205" s="99"/>
-      <c r="R205" s="99"/>
-      <c r="S205" s="99"/>
-      <c r="T205" s="99"/>
-      <c r="U205" s="99"/>
-      <c r="V205" s="99"/>
-      <c r="W205" s="99"/>
-      <c r="X205" s="99"/>
-      <c r="Y205" s="99"/>
-      <c r="Z205" s="99"/>
-      <c r="AA205" s="99"/>
-      <c r="AB205" s="99"/>
-      <c r="AC205" s="99"/>
-      <c r="AD205" s="99"/>
-      <c r="AE205" s="99"/>
-      <c r="AF205" s="99"/>
-      <c r="AG205" s="99"/>
-      <c r="AH205" s="99"/>
-      <c r="AI205" s="99"/>
-      <c r="AJ205" s="99"/>
-      <c r="AK205" s="99"/>
+      <c r="C205" s="100"/>
+      <c r="D205" s="100"/>
+      <c r="E205" s="100"/>
+      <c r="F205" s="100"/>
+      <c r="G205" s="100"/>
+      <c r="H205" s="100"/>
+      <c r="I205" s="100"/>
+      <c r="J205" s="100"/>
+      <c r="K205" s="100"/>
+      <c r="L205" s="100"/>
+      <c r="M205" s="100"/>
+      <c r="N205" s="100"/>
+      <c r="O205" s="100"/>
+      <c r="P205" s="100"/>
+      <c r="Q205" s="100"/>
+      <c r="R205" s="100"/>
+      <c r="S205" s="100"/>
+      <c r="T205" s="100"/>
+      <c r="U205" s="100"/>
+      <c r="V205" s="100"/>
+      <c r="W205" s="100"/>
+      <c r="X205" s="100"/>
+      <c r="Y205" s="100"/>
+      <c r="Z205" s="100"/>
+      <c r="AA205" s="100"/>
+      <c r="AB205" s="100"/>
+      <c r="AC205" s="100"/>
+      <c r="AD205" s="100"/>
+      <c r="AE205" s="100"/>
+      <c r="AF205" s="100"/>
+      <c r="AG205" s="100"/>
+      <c r="AH205" s="100"/>
+      <c r="AI205" s="100"/>
+      <c r="AJ205" s="100"/>
+      <c r="AK205" s="100"/>
     </row>
     <row r="206" spans="1:37" ht="15" customHeight="1">
       <c r="B206" s="15" t="s">
@@ -36839,7 +36803,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AK107"/>
   <sheetViews>
     <sheetView topLeftCell="Q1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
@@ -44032,42 +43996,42 @@
     </row>
     <row r="87" spans="1:37" ht="15" customHeight="1">
       <c r="A87" s="21"/>
-      <c r="B87" s="99" t="s">
+      <c r="B87" s="100" t="s">
         <v>7</v>
       </c>
-      <c r="C87" s="99"/>
-      <c r="D87" s="99"/>
-      <c r="E87" s="99"/>
-      <c r="F87" s="99"/>
-      <c r="G87" s="99"/>
-      <c r="H87" s="99"/>
-      <c r="I87" s="99"/>
-      <c r="J87" s="99"/>
-      <c r="K87" s="99"/>
-      <c r="L87" s="99"/>
-      <c r="M87" s="99"/>
-      <c r="N87" s="99"/>
-      <c r="O87" s="99"/>
-      <c r="P87" s="99"/>
-      <c r="Q87" s="99"/>
-      <c r="R87" s="99"/>
-      <c r="S87" s="99"/>
-      <c r="T87" s="99"/>
-      <c r="U87" s="99"/>
-      <c r="V87" s="99"/>
-      <c r="W87" s="99"/>
-      <c r="X87" s="99"/>
-      <c r="Y87" s="99"/>
-      <c r="Z87" s="99"/>
-      <c r="AA87" s="99"/>
-      <c r="AB87" s="99"/>
-      <c r="AC87" s="99"/>
-      <c r="AD87" s="99"/>
-      <c r="AE87" s="99"/>
-      <c r="AF87" s="99"/>
-      <c r="AG87" s="99"/>
-      <c r="AH87" s="99"/>
-      <c r="AI87" s="99"/>
+      <c r="C87" s="100"/>
+      <c r="D87" s="100"/>
+      <c r="E87" s="100"/>
+      <c r="F87" s="100"/>
+      <c r="G87" s="100"/>
+      <c r="H87" s="100"/>
+      <c r="I87" s="100"/>
+      <c r="J87" s="100"/>
+      <c r="K87" s="100"/>
+      <c r="L87" s="100"/>
+      <c r="M87" s="100"/>
+      <c r="N87" s="100"/>
+      <c r="O87" s="100"/>
+      <c r="P87" s="100"/>
+      <c r="Q87" s="100"/>
+      <c r="R87" s="100"/>
+      <c r="S87" s="100"/>
+      <c r="T87" s="100"/>
+      <c r="U87" s="100"/>
+      <c r="V87" s="100"/>
+      <c r="W87" s="100"/>
+      <c r="X87" s="100"/>
+      <c r="Y87" s="100"/>
+      <c r="Z87" s="100"/>
+      <c r="AA87" s="100"/>
+      <c r="AB87" s="100"/>
+      <c r="AC87" s="100"/>
+      <c r="AD87" s="100"/>
+      <c r="AE87" s="100"/>
+      <c r="AF87" s="100"/>
+      <c r="AG87" s="100"/>
+      <c r="AH87" s="100"/>
+      <c r="AI87" s="100"/>
       <c r="AJ87" s="18"/>
       <c r="AK87" s="18"/>
     </row>
@@ -44464,7 +44428,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ91"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -50812,42 +50776,42 @@
     </row>
     <row r="76" spans="1:36">
       <c r="A76" s="38"/>
-      <c r="B76" s="99" t="s">
+      <c r="B76" s="100" t="s">
         <v>446</v>
       </c>
-      <c r="C76" s="99"/>
-      <c r="D76" s="99"/>
-      <c r="E76" s="99"/>
-      <c r="F76" s="99"/>
-      <c r="G76" s="99"/>
-      <c r="H76" s="99"/>
-      <c r="I76" s="99"/>
-      <c r="J76" s="99"/>
-      <c r="K76" s="99"/>
-      <c r="L76" s="99"/>
-      <c r="M76" s="99"/>
-      <c r="N76" s="99"/>
-      <c r="O76" s="99"/>
-      <c r="P76" s="99"/>
-      <c r="Q76" s="99"/>
-      <c r="R76" s="99"/>
-      <c r="S76" s="99"/>
-      <c r="T76" s="99"/>
-      <c r="U76" s="99"/>
-      <c r="V76" s="99"/>
-      <c r="W76" s="99"/>
-      <c r="X76" s="99"/>
-      <c r="Y76" s="99"/>
-      <c r="Z76" s="99"/>
-      <c r="AA76" s="99"/>
-      <c r="AB76" s="99"/>
-      <c r="AC76" s="99"/>
-      <c r="AD76" s="99"/>
-      <c r="AE76" s="99"/>
-      <c r="AF76" s="99"/>
-      <c r="AG76" s="99"/>
-      <c r="AH76" s="99"/>
-      <c r="AI76" s="99"/>
+      <c r="C76" s="100"/>
+      <c r="D76" s="100"/>
+      <c r="E76" s="100"/>
+      <c r="F76" s="100"/>
+      <c r="G76" s="100"/>
+      <c r="H76" s="100"/>
+      <c r="I76" s="100"/>
+      <c r="J76" s="100"/>
+      <c r="K76" s="100"/>
+      <c r="L76" s="100"/>
+      <c r="M76" s="100"/>
+      <c r="N76" s="100"/>
+      <c r="O76" s="100"/>
+      <c r="P76" s="100"/>
+      <c r="Q76" s="100"/>
+      <c r="R76" s="100"/>
+      <c r="S76" s="100"/>
+      <c r="T76" s="100"/>
+      <c r="U76" s="100"/>
+      <c r="V76" s="100"/>
+      <c r="W76" s="100"/>
+      <c r="X76" s="100"/>
+      <c r="Y76" s="100"/>
+      <c r="Z76" s="100"/>
+      <c r="AA76" s="100"/>
+      <c r="AB76" s="100"/>
+      <c r="AC76" s="100"/>
+      <c r="AD76" s="100"/>
+      <c r="AE76" s="100"/>
+      <c r="AF76" s="100"/>
+      <c r="AG76" s="100"/>
+      <c r="AH76" s="100"/>
+      <c r="AI76" s="100"/>
       <c r="AJ76" s="37"/>
     </row>
     <row r="77" spans="1:36">
@@ -51063,7 +51027,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AK214"/>
   <sheetViews>
     <sheetView topLeftCell="A67" workbookViewId="0">
@@ -70074,42 +70038,42 @@
     </row>
     <row r="205" spans="1:37" ht="15" customHeight="1">
       <c r="A205" s="53"/>
-      <c r="B205" s="99" t="s">
+      <c r="B205" s="100" t="s">
         <v>388</v>
       </c>
-      <c r="C205" s="99"/>
-      <c r="D205" s="99"/>
-      <c r="E205" s="99"/>
-      <c r="F205" s="99"/>
-      <c r="G205" s="99"/>
-      <c r="H205" s="99"/>
-      <c r="I205" s="99"/>
-      <c r="J205" s="99"/>
-      <c r="K205" s="99"/>
-      <c r="L205" s="99"/>
-      <c r="M205" s="99"/>
-      <c r="N205" s="99"/>
-      <c r="O205" s="99"/>
-      <c r="P205" s="99"/>
-      <c r="Q205" s="99"/>
-      <c r="R205" s="99"/>
-      <c r="S205" s="99"/>
-      <c r="T205" s="99"/>
-      <c r="U205" s="99"/>
-      <c r="V205" s="99"/>
-      <c r="W205" s="99"/>
-      <c r="X205" s="99"/>
-      <c r="Y205" s="99"/>
-      <c r="Z205" s="99"/>
-      <c r="AA205" s="99"/>
-      <c r="AB205" s="99"/>
-      <c r="AC205" s="99"/>
-      <c r="AD205" s="99"/>
-      <c r="AE205" s="99"/>
-      <c r="AF205" s="99"/>
-      <c r="AG205" s="99"/>
-      <c r="AH205" s="99"/>
-      <c r="AI205" s="99"/>
+      <c r="C205" s="100"/>
+      <c r="D205" s="100"/>
+      <c r="E205" s="100"/>
+      <c r="F205" s="100"/>
+      <c r="G205" s="100"/>
+      <c r="H205" s="100"/>
+      <c r="I205" s="100"/>
+      <c r="J205" s="100"/>
+      <c r="K205" s="100"/>
+      <c r="L205" s="100"/>
+      <c r="M205" s="100"/>
+      <c r="N205" s="100"/>
+      <c r="O205" s="100"/>
+      <c r="P205" s="100"/>
+      <c r="Q205" s="100"/>
+      <c r="R205" s="100"/>
+      <c r="S205" s="100"/>
+      <c r="T205" s="100"/>
+      <c r="U205" s="100"/>
+      <c r="V205" s="100"/>
+      <c r="W205" s="100"/>
+      <c r="X205" s="100"/>
+      <c r="Y205" s="100"/>
+      <c r="Z205" s="100"/>
+      <c r="AA205" s="100"/>
+      <c r="AB205" s="100"/>
+      <c r="AC205" s="100"/>
+      <c r="AD205" s="100"/>
+      <c r="AE205" s="100"/>
+      <c r="AF205" s="100"/>
+      <c r="AG205" s="100"/>
+      <c r="AH205" s="100"/>
+      <c r="AI205" s="100"/>
       <c r="AJ205" s="52"/>
       <c r="AK205" s="52"/>
     </row>
@@ -70264,7 +70228,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -71217,14 +71181,14 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
-  <dimension ref="A1:AI7"/>
+  <dimension ref="A1:AJ7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C6" sqref="C6:G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -71232,7 +71196,7 @@
     <col min="1" max="1" width="16.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" ht="71.25">
+    <row r="1" spans="1:36" ht="71.25">
       <c r="A1" s="19" t="s">
         <v>455</v>
       </c>
@@ -71243,127 +71207,130 @@
         <v>2019</v>
       </c>
       <c r="D1">
+        <v>2020</v>
+      </c>
+      <c r="E1">
         <f>'AEO 2020 7'!E1</f>
         <v>2021</v>
       </c>
-      <c r="E1">
+      <c r="F1">
         <f>'AEO 2020 7'!F1</f>
         <v>2022</v>
       </c>
-      <c r="F1">
+      <c r="G1">
         <f>'AEO 2020 7'!G1</f>
         <v>2023</v>
       </c>
-      <c r="G1">
+      <c r="H1">
         <f>'AEO 2020 7'!H1</f>
         <v>2024</v>
       </c>
-      <c r="H1">
+      <c r="I1">
         <f>'AEO 2020 7'!I1</f>
         <v>2025</v>
       </c>
-      <c r="I1">
+      <c r="J1">
         <f>'AEO 2020 7'!J1</f>
         <v>2026</v>
       </c>
-      <c r="J1">
+      <c r="K1">
         <f>'AEO 2020 7'!K1</f>
         <v>2027</v>
       </c>
-      <c r="K1">
+      <c r="L1">
         <f>'AEO 2020 7'!L1</f>
         <v>2028</v>
       </c>
-      <c r="L1">
+      <c r="M1">
         <f>'AEO 2020 7'!M1</f>
         <v>2029</v>
       </c>
-      <c r="M1">
+      <c r="N1">
         <f>'AEO 2020 7'!N1</f>
         <v>2030</v>
       </c>
-      <c r="N1">
+      <c r="O1">
         <f>'AEO 2020 7'!O1</f>
         <v>2031</v>
       </c>
-      <c r="O1">
+      <c r="P1">
         <f>'AEO 2020 7'!P1</f>
         <v>2032</v>
       </c>
-      <c r="P1">
+      <c r="Q1">
         <f>'AEO 2020 7'!Q1</f>
         <v>2033</v>
       </c>
-      <c r="Q1">
+      <c r="R1">
         <f>'AEO 2020 7'!R1</f>
         <v>2034</v>
       </c>
-      <c r="R1">
+      <c r="S1">
         <f>'AEO 2020 7'!S1</f>
         <v>2035</v>
       </c>
-      <c r="S1">
+      <c r="T1">
         <f>'AEO 2020 7'!T1</f>
         <v>2036</v>
       </c>
-      <c r="T1">
+      <c r="U1">
         <f>'AEO 2020 7'!U1</f>
         <v>2037</v>
       </c>
-      <c r="U1">
+      <c r="V1">
         <f>'AEO 2020 7'!V1</f>
         <v>2038</v>
       </c>
-      <c r="V1">
+      <c r="W1">
         <f>'AEO 2020 7'!W1</f>
         <v>2039</v>
       </c>
-      <c r="W1">
+      <c r="X1">
         <f>'AEO 2020 7'!X1</f>
         <v>2040</v>
       </c>
-      <c r="X1">
+      <c r="Y1">
         <f>'AEO 2020 7'!Y1</f>
         <v>2041</v>
       </c>
-      <c r="Y1">
+      <c r="Z1">
         <f>'AEO 2020 7'!Z1</f>
         <v>2042</v>
       </c>
-      <c r="Z1">
+      <c r="AA1">
         <f>'AEO 2020 7'!AA1</f>
         <v>2043</v>
       </c>
-      <c r="AA1">
+      <c r="AB1">
         <f>'AEO 2020 7'!AB1</f>
         <v>2044</v>
       </c>
-      <c r="AB1">
+      <c r="AC1">
         <f>'AEO 2020 7'!AC1</f>
         <v>2045</v>
       </c>
-      <c r="AC1">
+      <c r="AD1">
         <f>'AEO 2020 7'!AD1</f>
         <v>2046</v>
       </c>
-      <c r="AD1">
+      <c r="AE1">
         <f>'AEO 2020 7'!AE1</f>
         <v>2047</v>
       </c>
-      <c r="AE1">
+      <c r="AF1">
         <f>'AEO 2020 7'!AF1</f>
         <v>2048</v>
       </c>
-      <c r="AF1">
+      <c r="AG1">
         <f>'AEO 2020 7'!AG1</f>
         <v>2049</v>
       </c>
-      <c r="AG1">
+      <c r="AH1">
         <f>'AEO 2020 7'!AH1</f>
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:35">
+    <row r="2" spans="1:36">
       <c r="A2" t="s">
         <v>372</v>
       </c>
@@ -71377,128 +71344,132 @@
       </c>
       <c r="D2" s="12">
         <f>INDEX('AEO 2020 7'!19:19,MATCH(D$1,'AEO 2020 7'!1:1,0))/INDEX('AEO 2019 7'!19:19,MATCH($B$1,'AEO 2019 7'!1:1,0))</f>
-        <v>1.0180380615275557</v>
+        <v>1.0086119840394017</v>
       </c>
       <c r="E2" s="12">
         <f>INDEX('AEO 2020 7'!19:19,MATCH(E$1,'AEO 2020 7'!1:1,0))/INDEX('AEO 2019 7'!19:19,MATCH($B$1,'AEO 2019 7'!1:1,0))</f>
-        <v>1.0306452815933418</v>
+        <v>1.0180380615275557</v>
       </c>
       <c r="F2" s="12">
         <f>INDEX('AEO 2020 7'!19:19,MATCH(F$1,'AEO 2020 7'!1:1,0))/INDEX('AEO 2019 7'!19:19,MATCH($B$1,'AEO 2019 7'!1:1,0))</f>
-        <v>1.0400992742459336</v>
+        <v>1.0306452815933418</v>
       </c>
       <c r="G2" s="12">
         <f>INDEX('AEO 2020 7'!19:19,MATCH(G$1,'AEO 2020 7'!1:1,0))/INDEX('AEO 2019 7'!19:19,MATCH($B$1,'AEO 2019 7'!1:1,0))</f>
-        <v>1.0504304785746841</v>
+        <v>1.0400992742459336</v>
       </c>
       <c r="H2" s="12">
         <f>INDEX('AEO 2020 7'!19:19,MATCH(H$1,'AEO 2020 7'!1:1,0))/INDEX('AEO 2019 7'!19:19,MATCH($B$1,'AEO 2019 7'!1:1,0))</f>
-        <v>1.0609741276586506</v>
+        <v>1.0504304785746841</v>
       </c>
       <c r="I2" s="12">
         <f>INDEX('AEO 2020 7'!19:19,MATCH(I$1,'AEO 2020 7'!1:1,0))/INDEX('AEO 2019 7'!19:19,MATCH($B$1,'AEO 2019 7'!1:1,0))</f>
-        <v>1.0732324634564665</v>
+        <v>1.0609741276586506</v>
       </c>
       <c r="J2" s="12">
         <f>INDEX('AEO 2020 7'!19:19,MATCH(J$1,'AEO 2020 7'!1:1,0))/INDEX('AEO 2019 7'!19:19,MATCH($B$1,'AEO 2019 7'!1:1,0))</f>
-        <v>1.0861365573254036</v>
+        <v>1.0732324634564665</v>
       </c>
       <c r="K2" s="12">
         <f>INDEX('AEO 2020 7'!19:19,MATCH(K$1,'AEO 2020 7'!1:1,0))/INDEX('AEO 2019 7'!19:19,MATCH($B$1,'AEO 2019 7'!1:1,0))</f>
-        <v>1.1004604645075322</v>
+        <v>1.0861365573254036</v>
       </c>
       <c r="L2" s="12">
         <f>INDEX('AEO 2020 7'!19:19,MATCH(L$1,'AEO 2020 7'!1:1,0))/INDEX('AEO 2019 7'!19:19,MATCH($B$1,'AEO 2019 7'!1:1,0))</f>
-        <v>1.1149171320701914</v>
+        <v>1.1004604645075322</v>
       </c>
       <c r="M2" s="12">
         <f>INDEX('AEO 2020 7'!19:19,MATCH(M$1,'AEO 2020 7'!1:1,0))/INDEX('AEO 2019 7'!19:19,MATCH($B$1,'AEO 2019 7'!1:1,0))</f>
-        <v>1.1301056755339114</v>
+        <v>1.1149171320701914</v>
       </c>
       <c r="N2" s="12">
         <f>INDEX('AEO 2020 7'!19:19,MATCH(N$1,'AEO 2020 7'!1:1,0))/INDEX('AEO 2019 7'!19:19,MATCH($B$1,'AEO 2019 7'!1:1,0))</f>
-        <v>1.1460106043447134</v>
+        <v>1.1301056755339114</v>
       </c>
       <c r="O2" s="12">
         <f>INDEX('AEO 2020 7'!19:19,MATCH(O$1,'AEO 2020 7'!1:1,0))/INDEX('AEO 2019 7'!19:19,MATCH($B$1,'AEO 2019 7'!1:1,0))</f>
-        <v>1.1602650201578248</v>
+        <v>1.1460106043447134</v>
       </c>
       <c r="P2" s="12">
         <f>INDEX('AEO 2020 7'!19:19,MATCH(P$1,'AEO 2020 7'!1:1,0))/INDEX('AEO 2019 7'!19:19,MATCH($B$1,'AEO 2019 7'!1:1,0))</f>
-        <v>1.1747221501250804</v>
+        <v>1.1602650201578248</v>
       </c>
       <c r="Q2" s="12">
         <f>INDEX('AEO 2020 7'!19:19,MATCH(Q$1,'AEO 2020 7'!1:1,0))/INDEX('AEO 2019 7'!19:19,MATCH($B$1,'AEO 2019 7'!1:1,0))</f>
-        <v>1.1903841858432218</v>
+        <v>1.1747221501250804</v>
       </c>
       <c r="R2" s="12">
         <f>INDEX('AEO 2020 7'!19:19,MATCH(R$1,'AEO 2020 7'!1:1,0))/INDEX('AEO 2019 7'!19:19,MATCH($B$1,'AEO 2019 7'!1:1,0))</f>
-        <v>1.2051611992684357</v>
+        <v>1.1903841858432218</v>
       </c>
       <c r="S2" s="12">
         <f>INDEX('AEO 2020 7'!19:19,MATCH(S$1,'AEO 2020 7'!1:1,0))/INDEX('AEO 2019 7'!19:19,MATCH($B$1,'AEO 2019 7'!1:1,0))</f>
-        <v>1.2194320304447186</v>
+        <v>1.2051611992684357</v>
       </c>
       <c r="T2" s="12">
         <f>INDEX('AEO 2020 7'!19:19,MATCH(T$1,'AEO 2020 7'!1:1,0))/INDEX('AEO 2019 7'!19:19,MATCH($B$1,'AEO 2019 7'!1:1,0))</f>
-        <v>1.2336987301364557</v>
+        <v>1.2194320304447186</v>
       </c>
       <c r="U2" s="12">
         <f>INDEX('AEO 2020 7'!19:19,MATCH(U$1,'AEO 2020 7'!1:1,0))/INDEX('AEO 2019 7'!19:19,MATCH($B$1,'AEO 2019 7'!1:1,0))</f>
-        <v>1.2476203051106363</v>
+        <v>1.2336987301364557</v>
       </c>
       <c r="V2" s="12">
         <f>INDEX('AEO 2020 7'!19:19,MATCH(V$1,'AEO 2020 7'!1:1,0))/INDEX('AEO 2019 7'!19:19,MATCH($B$1,'AEO 2019 7'!1:1,0))</f>
-        <v>1.2614826721919326</v>
+        <v>1.2476203051106363</v>
       </c>
       <c r="W2" s="12">
         <f>INDEX('AEO 2020 7'!19:19,MATCH(W$1,'AEO 2020 7'!1:1,0))/INDEX('AEO 2019 7'!19:19,MATCH($B$1,'AEO 2019 7'!1:1,0))</f>
-        <v>1.2768893298933113</v>
+        <v>1.2614826721919326</v>
       </c>
       <c r="X2" s="12">
         <f>INDEX('AEO 2020 7'!19:19,MATCH(X$1,'AEO 2020 7'!1:1,0))/INDEX('AEO 2019 7'!19:19,MATCH($B$1,'AEO 2019 7'!1:1,0))</f>
-        <v>1.2930764863442876</v>
+        <v>1.2768893298933113</v>
       </c>
       <c r="Y2" s="12">
         <f>INDEX('AEO 2020 7'!19:19,MATCH(Y$1,'AEO 2020 7'!1:1,0))/INDEX('AEO 2019 7'!19:19,MATCH($B$1,'AEO 2019 7'!1:1,0))</f>
-        <v>1.3087802490511156</v>
+        <v>1.2930764863442876</v>
       </c>
       <c r="Z2" s="12">
         <f>INDEX('AEO 2020 7'!19:19,MATCH(Z$1,'AEO 2020 7'!1:1,0))/INDEX('AEO 2019 7'!19:19,MATCH($B$1,'AEO 2019 7'!1:1,0))</f>
-        <v>1.3256503569864009</v>
+        <v>1.3087802490511156</v>
       </c>
       <c r="AA2" s="12">
         <f>INDEX('AEO 2020 7'!19:19,MATCH(AA$1,'AEO 2020 7'!1:1,0))/INDEX('AEO 2019 7'!19:19,MATCH($B$1,'AEO 2019 7'!1:1,0))</f>
-        <v>1.3428941179923841</v>
+        <v>1.3256503569864009</v>
       </c>
       <c r="AB2" s="12">
         <f>INDEX('AEO 2020 7'!19:19,MATCH(AB$1,'AEO 2020 7'!1:1,0))/INDEX('AEO 2019 7'!19:19,MATCH($B$1,'AEO 2019 7'!1:1,0))</f>
-        <v>1.3602240671942236</v>
+        <v>1.3428941179923841</v>
       </c>
       <c r="AC2" s="12">
         <f>INDEX('AEO 2020 7'!19:19,MATCH(AC$1,'AEO 2020 7'!1:1,0))/INDEX('AEO 2019 7'!19:19,MATCH($B$1,'AEO 2019 7'!1:1,0))</f>
-        <v>1.377615687096037</v>
+        <v>1.3602240671942236</v>
       </c>
       <c r="AD2" s="12">
         <f>INDEX('AEO 2020 7'!19:19,MATCH(AD$1,'AEO 2020 7'!1:1,0))/INDEX('AEO 2019 7'!19:19,MATCH($B$1,'AEO 2019 7'!1:1,0))</f>
-        <v>1.3951912133476505</v>
+        <v>1.377615687096037</v>
       </c>
       <c r="AE2" s="12">
         <f>INDEX('AEO 2020 7'!19:19,MATCH(AE$1,'AEO 2020 7'!1:1,0))/INDEX('AEO 2019 7'!19:19,MATCH($B$1,'AEO 2019 7'!1:1,0))</f>
-        <v>1.4121450768285237</v>
+        <v>1.3951912133476505</v>
       </c>
       <c r="AF2" s="12">
         <f>INDEX('AEO 2020 7'!19:19,MATCH(AF$1,'AEO 2020 7'!1:1,0))/INDEX('AEO 2019 7'!19:19,MATCH($B$1,'AEO 2019 7'!1:1,0))</f>
-        <v>1.4297940751495928</v>
+        <v>1.4121450768285237</v>
       </c>
       <c r="AG2" s="12">
         <f>INDEX('AEO 2020 7'!19:19,MATCH(AG$1,'AEO 2020 7'!1:1,0))/INDEX('AEO 2019 7'!19:19,MATCH($B$1,'AEO 2019 7'!1:1,0))</f>
+        <v>1.4297940751495928</v>
+      </c>
+      <c r="AH2" s="12">
+        <f>INDEX('AEO 2020 7'!19:19,MATCH(AH$1,'AEO 2020 7'!1:1,0))/INDEX('AEO 2019 7'!19:19,MATCH($B$1,'AEO 2019 7'!1:1,0))</f>
         <v>1.4468872028321678</v>
       </c>
-      <c r="AH2" s="12"/>
       <c r="AI2" s="12"/>
-    </row>
-    <row r="3" spans="1:35">
+      <c r="AJ2" s="12"/>
+    </row>
+    <row r="3" spans="1:36">
       <c r="A3" t="s">
         <v>370</v>
       </c>
@@ -71512,128 +71483,132 @@
       </c>
       <c r="D3" s="12">
         <f>INDEX('AEO 2020 7'!20:20,MATCH(D$1,'AEO 2020 7'!1:1,0))/INDEX('AEO 2019 7'!20:20,MATCH($B$1,'AEO 2019 7'!1:1,0))</f>
-        <v>1.0203735565555867</v>
+        <v>1.0145500621583856</v>
       </c>
       <c r="E3" s="12">
         <f>INDEX('AEO 2020 7'!20:20,MATCH(E$1,'AEO 2020 7'!1:1,0))/INDEX('AEO 2019 7'!20:20,MATCH($B$1,'AEO 2019 7'!1:1,0))</f>
-        <v>1.0337918591970117</v>
+        <v>1.0203735565555867</v>
       </c>
       <c r="F3" s="12">
         <f>INDEX('AEO 2020 7'!20:20,MATCH(F$1,'AEO 2020 7'!1:1,0))/INDEX('AEO 2019 7'!20:20,MATCH($B$1,'AEO 2019 7'!1:1,0))</f>
-        <v>1.0456067261636848</v>
+        <v>1.0337918591970117</v>
       </c>
       <c r="G3" s="12">
         <f>INDEX('AEO 2020 7'!20:20,MATCH(G$1,'AEO 2020 7'!1:1,0))/INDEX('AEO 2019 7'!20:20,MATCH($B$1,'AEO 2019 7'!1:1,0))</f>
-        <v>1.0577322756459737</v>
+        <v>1.0456067261636848</v>
       </c>
       <c r="H3" s="12">
         <f>INDEX('AEO 2020 7'!20:20,MATCH(H$1,'AEO 2020 7'!1:1,0))/INDEX('AEO 2019 7'!20:20,MATCH($B$1,'AEO 2019 7'!1:1,0))</f>
-        <v>1.0685307570472358</v>
+        <v>1.0577322756459737</v>
       </c>
       <c r="I3" s="12">
         <f>INDEX('AEO 2020 7'!20:20,MATCH(I$1,'AEO 2020 7'!1:1,0))/INDEX('AEO 2019 7'!20:20,MATCH($B$1,'AEO 2019 7'!1:1,0))</f>
-        <v>1.0801805265858233</v>
+        <v>1.0685307570472358</v>
       </c>
       <c r="J3" s="12">
         <f>INDEX('AEO 2020 7'!20:20,MATCH(J$1,'AEO 2020 7'!1:1,0))/INDEX('AEO 2019 7'!20:20,MATCH($B$1,'AEO 2019 7'!1:1,0))</f>
-        <v>1.0905733963860682</v>
+        <v>1.0801805265858233</v>
       </c>
       <c r="K3" s="12">
         <f>INDEX('AEO 2020 7'!20:20,MATCH(K$1,'AEO 2020 7'!1:1,0))/INDEX('AEO 2019 7'!20:20,MATCH($B$1,'AEO 2019 7'!1:1,0))</f>
-        <v>1.1026016534870502</v>
+        <v>1.0905733963860682</v>
       </c>
       <c r="L3" s="12">
         <f>INDEX('AEO 2020 7'!20:20,MATCH(L$1,'AEO 2020 7'!1:1,0))/INDEX('AEO 2019 7'!20:20,MATCH($B$1,'AEO 2019 7'!1:1,0))</f>
-        <v>1.1144931659777795</v>
+        <v>1.1026016534870502</v>
       </c>
       <c r="M3" s="12">
         <f>INDEX('AEO 2020 7'!20:20,MATCH(M$1,'AEO 2020 7'!1:1,0))/INDEX('AEO 2019 7'!20:20,MATCH($B$1,'AEO 2019 7'!1:1,0))</f>
-        <v>1.1271204849256968</v>
+        <v>1.1144931659777795</v>
       </c>
       <c r="N3" s="12">
         <f>INDEX('AEO 2020 7'!20:20,MATCH(N$1,'AEO 2020 7'!1:1,0))/INDEX('AEO 2019 7'!20:20,MATCH($B$1,'AEO 2019 7'!1:1,0))</f>
-        <v>1.1404393338810122</v>
+        <v>1.1271204849256968</v>
       </c>
       <c r="O3" s="12">
         <f>INDEX('AEO 2020 7'!20:20,MATCH(O$1,'AEO 2020 7'!1:1,0))/INDEX('AEO 2019 7'!20:20,MATCH($B$1,'AEO 2019 7'!1:1,0))</f>
-        <v>1.1533956222724089</v>
+        <v>1.1404393338810122</v>
       </c>
       <c r="P3" s="12">
         <f>INDEX('AEO 2020 7'!20:20,MATCH(P$1,'AEO 2020 7'!1:1,0))/INDEX('AEO 2019 7'!20:20,MATCH($B$1,'AEO 2019 7'!1:1,0))</f>
-        <v>1.1661336963086524</v>
+        <v>1.1533956222724089</v>
       </c>
       <c r="Q3" s="12">
         <f>INDEX('AEO 2020 7'!20:20,MATCH(Q$1,'AEO 2020 7'!1:1,0))/INDEX('AEO 2019 7'!20:20,MATCH($B$1,'AEO 2019 7'!1:1,0))</f>
-        <v>1.1808441293033121</v>
+        <v>1.1661336963086524</v>
       </c>
       <c r="R3" s="12">
         <f>INDEX('AEO 2020 7'!20:20,MATCH(R$1,'AEO 2020 7'!1:1,0))/INDEX('AEO 2019 7'!20:20,MATCH($B$1,'AEO 2019 7'!1:1,0))</f>
-        <v>1.1945834867034946</v>
+        <v>1.1808441293033121</v>
       </c>
       <c r="S3" s="12">
         <f>INDEX('AEO 2020 7'!20:20,MATCH(S$1,'AEO 2020 7'!1:1,0))/INDEX('AEO 2019 7'!20:20,MATCH($B$1,'AEO 2019 7'!1:1,0))</f>
-        <v>1.2065243119555176</v>
+        <v>1.1945834867034946</v>
       </c>
       <c r="T3" s="12">
         <f>INDEX('AEO 2020 7'!20:20,MATCH(T$1,'AEO 2020 7'!1:1,0))/INDEX('AEO 2019 7'!20:20,MATCH($B$1,'AEO 2019 7'!1:1,0))</f>
-        <v>1.2182223674672916</v>
+        <v>1.2065243119555176</v>
       </c>
       <c r="U3" s="12">
         <f>INDEX('AEO 2020 7'!20:20,MATCH(U$1,'AEO 2020 7'!1:1,0))/INDEX('AEO 2019 7'!20:20,MATCH($B$1,'AEO 2019 7'!1:1,0))</f>
-        <v>1.2298944300906203</v>
+        <v>1.2182223674672916</v>
       </c>
       <c r="V3" s="12">
         <f>INDEX('AEO 2020 7'!20:20,MATCH(V$1,'AEO 2020 7'!1:1,0))/INDEX('AEO 2019 7'!20:20,MATCH($B$1,'AEO 2019 7'!1:1,0))</f>
-        <v>1.2411880085180726</v>
+        <v>1.2298944300906203</v>
       </c>
       <c r="W3" s="12">
         <f>INDEX('AEO 2020 7'!20:20,MATCH(W$1,'AEO 2020 7'!1:1,0))/INDEX('AEO 2019 7'!20:20,MATCH($B$1,'AEO 2019 7'!1:1,0))</f>
-        <v>1.2550285600943698</v>
+        <v>1.2411880085180726</v>
       </c>
       <c r="X3" s="12">
         <f>INDEX('AEO 2020 7'!20:20,MATCH(X$1,'AEO 2020 7'!1:1,0))/INDEX('AEO 2019 7'!20:20,MATCH($B$1,'AEO 2019 7'!1:1,0))</f>
-        <v>1.2693793108983296</v>
+        <v>1.2550285600943698</v>
       </c>
       <c r="Y3" s="12">
         <f>INDEX('AEO 2020 7'!20:20,MATCH(Y$1,'AEO 2020 7'!1:1,0))/INDEX('AEO 2019 7'!20:20,MATCH($B$1,'AEO 2019 7'!1:1,0))</f>
-        <v>1.2828644927939776</v>
+        <v>1.2693793108983296</v>
       </c>
       <c r="Z3" s="12">
         <f>INDEX('AEO 2020 7'!20:20,MATCH(Z$1,'AEO 2020 7'!1:1,0))/INDEX('AEO 2019 7'!20:20,MATCH($B$1,'AEO 2019 7'!1:1,0))</f>
-        <v>1.2973032915197611</v>
+        <v>1.2828644927939776</v>
       </c>
       <c r="AA3" s="12">
         <f>INDEX('AEO 2020 7'!20:20,MATCH(AA$1,'AEO 2020 7'!1:1,0))/INDEX('AEO 2019 7'!20:20,MATCH($B$1,'AEO 2019 7'!1:1,0))</f>
-        <v>1.3119705758482887</v>
+        <v>1.2973032915197611</v>
       </c>
       <c r="AB3" s="12">
         <f>INDEX('AEO 2020 7'!20:20,MATCH(AB$1,'AEO 2020 7'!1:1,0))/INDEX('AEO 2019 7'!20:20,MATCH($B$1,'AEO 2019 7'!1:1,0))</f>
-        <v>1.3267866266242199</v>
+        <v>1.3119705758482887</v>
       </c>
       <c r="AC3" s="12">
         <f>INDEX('AEO 2020 7'!20:20,MATCH(AC$1,'AEO 2020 7'!1:1,0))/INDEX('AEO 2019 7'!20:20,MATCH($B$1,'AEO 2019 7'!1:1,0))</f>
-        <v>1.341054776533102</v>
+        <v>1.3267866266242199</v>
       </c>
       <c r="AD3" s="12">
         <f>INDEX('AEO 2020 7'!20:20,MATCH(AD$1,'AEO 2020 7'!1:1,0))/INDEX('AEO 2019 7'!20:20,MATCH($B$1,'AEO 2019 7'!1:1,0))</f>
-        <v>1.3556160357316338</v>
+        <v>1.341054776533102</v>
       </c>
       <c r="AE3" s="12">
         <f>INDEX('AEO 2020 7'!20:20,MATCH(AE$1,'AEO 2020 7'!1:1,0))/INDEX('AEO 2019 7'!20:20,MATCH($B$1,'AEO 2019 7'!1:1,0))</f>
-        <v>1.3695320006862581</v>
+        <v>1.3556160357316338</v>
       </c>
       <c r="AF3" s="12">
         <f>INDEX('AEO 2020 7'!20:20,MATCH(AF$1,'AEO 2020 7'!1:1,0))/INDEX('AEO 2019 7'!20:20,MATCH($B$1,'AEO 2019 7'!1:1,0))</f>
-        <v>1.38406069218594</v>
+        <v>1.3695320006862581</v>
       </c>
       <c r="AG3" s="12">
         <f>INDEX('AEO 2020 7'!20:20,MATCH(AG$1,'AEO 2020 7'!1:1,0))/INDEX('AEO 2019 7'!20:20,MATCH($B$1,'AEO 2019 7'!1:1,0))</f>
+        <v>1.38406069218594</v>
+      </c>
+      <c r="AH3" s="12">
+        <f>INDEX('AEO 2020 7'!20:20,MATCH(AH$1,'AEO 2020 7'!1:1,0))/INDEX('AEO 2019 7'!20:20,MATCH($B$1,'AEO 2019 7'!1:1,0))</f>
         <v>1.3969795852911238</v>
       </c>
-      <c r="AH3" s="16"/>
       <c r="AI3" s="16"/>
-    </row>
-    <row r="4" spans="1:35">
+      <c r="AJ3" s="16"/>
+    </row>
+    <row r="4" spans="1:36">
       <c r="A4" t="s">
         <v>367</v>
       </c>
@@ -71647,128 +71622,132 @@
       </c>
       <c r="D4" s="12">
         <f>INDEX('AEO 2020 47'!74:74,MATCH(D$1,'AEO 2020 47'!1:1,0))/INDEX('AEO 2019 48'!74:74,MATCH($B$1,'AEO 2019 48'!1:1,0))</f>
-        <v>1.0562664082758708</v>
+        <v>1.0834714425902596</v>
       </c>
       <c r="E4" s="12">
         <f>INDEX('AEO 2020 47'!74:74,MATCH(E$1,'AEO 2020 47'!1:1,0))/INDEX('AEO 2019 48'!74:74,MATCH($B$1,'AEO 2019 48'!1:1,0))</f>
-        <v>1.0538908222693684</v>
+        <v>1.0562664082758708</v>
       </c>
       <c r="F4" s="12">
         <f>INDEX('AEO 2020 47'!74:74,MATCH(F$1,'AEO 2020 47'!1:1,0))/INDEX('AEO 2019 48'!74:74,MATCH($B$1,'AEO 2019 48'!1:1,0))</f>
-        <v>1.0582489301853917</v>
+        <v>1.0538908222693684</v>
       </c>
       <c r="G4" s="12">
         <f>INDEX('AEO 2020 47'!74:74,MATCH(G$1,'AEO 2020 47'!1:1,0))/INDEX('AEO 2019 48'!74:74,MATCH($B$1,'AEO 2019 48'!1:1,0))</f>
-        <v>1.0725660280002827</v>
+        <v>1.0582489301853917</v>
       </c>
       <c r="H4" s="12">
         <f>INDEX('AEO 2020 47'!74:74,MATCH(H$1,'AEO 2020 47'!1:1,0))/INDEX('AEO 2019 48'!74:74,MATCH($B$1,'AEO 2019 48'!1:1,0))</f>
-        <v>1.0816777322911695</v>
+        <v>1.0725660280002827</v>
       </c>
       <c r="I4" s="12">
         <f>INDEX('AEO 2020 47'!74:74,MATCH(I$1,'AEO 2020 47'!1:1,0))/INDEX('AEO 2019 48'!74:74,MATCH($B$1,'AEO 2019 48'!1:1,0))</f>
-        <v>1.0999883890383864</v>
+        <v>1.0816777322911695</v>
       </c>
       <c r="J4" s="12">
         <f>INDEX('AEO 2020 47'!74:74,MATCH(J$1,'AEO 2020 47'!1:1,0))/INDEX('AEO 2019 48'!74:74,MATCH($B$1,'AEO 2019 48'!1:1,0))</f>
-        <v>1.1149987966218133</v>
+        <v>1.0999883890383864</v>
       </c>
       <c r="K4" s="12">
         <f>INDEX('AEO 2020 47'!74:74,MATCH(K$1,'AEO 2020 47'!1:1,0))/INDEX('AEO 2019 48'!74:74,MATCH($B$1,'AEO 2019 48'!1:1,0))</f>
-        <v>1.1293145668099724</v>
+        <v>1.1149987966218133</v>
       </c>
       <c r="L4" s="12">
         <f>INDEX('AEO 2020 47'!74:74,MATCH(L$1,'AEO 2020 47'!1:1,0))/INDEX('AEO 2019 48'!74:74,MATCH($B$1,'AEO 2019 48'!1:1,0))</f>
-        <v>1.1401157049785973</v>
+        <v>1.1293145668099724</v>
       </c>
       <c r="M4" s="12">
         <f>INDEX('AEO 2020 47'!74:74,MATCH(M$1,'AEO 2020 47'!1:1,0))/INDEX('AEO 2019 48'!74:74,MATCH($B$1,'AEO 2019 48'!1:1,0))</f>
-        <v>1.1461123063118868</v>
+        <v>1.1401157049785973</v>
       </c>
       <c r="N4" s="12">
         <f>INDEX('AEO 2020 47'!74:74,MATCH(N$1,'AEO 2020 47'!1:1,0))/INDEX('AEO 2019 48'!74:74,MATCH($B$1,'AEO 2019 48'!1:1,0))</f>
-        <v>1.1490054358522077</v>
+        <v>1.1461123063118868</v>
       </c>
       <c r="O4" s="12">
         <f>INDEX('AEO 2020 47'!74:74,MATCH(O$1,'AEO 2020 47'!1:1,0))/INDEX('AEO 2019 48'!74:74,MATCH($B$1,'AEO 2019 48'!1:1,0))</f>
-        <v>1.1524410452197458</v>
+        <v>1.1490054358522077</v>
       </c>
       <c r="P4" s="12">
         <f>INDEX('AEO 2020 47'!74:74,MATCH(P$1,'AEO 2020 47'!1:1,0))/INDEX('AEO 2019 48'!74:74,MATCH($B$1,'AEO 2019 48'!1:1,0))</f>
-        <v>1.1527386356378364</v>
+        <v>1.1524410452197458</v>
       </c>
       <c r="Q4" s="12">
         <f>INDEX('AEO 2020 47'!74:74,MATCH(Q$1,'AEO 2020 47'!1:1,0))/INDEX('AEO 2019 48'!74:74,MATCH($B$1,'AEO 2019 48'!1:1,0))</f>
-        <v>1.1565823747796176</v>
+        <v>1.1527386356378364</v>
       </c>
       <c r="R4" s="12">
         <f>INDEX('AEO 2020 47'!74:74,MATCH(R$1,'AEO 2020 47'!1:1,0))/INDEX('AEO 2019 48'!74:74,MATCH($B$1,'AEO 2019 48'!1:1,0))</f>
-        <v>1.1582531064373069</v>
+        <v>1.1565823747796176</v>
       </c>
       <c r="S4" s="12">
         <f>INDEX('AEO 2020 47'!74:74,MATCH(S$1,'AEO 2020 47'!1:1,0))/INDEX('AEO 2019 48'!74:74,MATCH($B$1,'AEO 2019 48'!1:1,0))</f>
-        <v>1.1566139492066752</v>
+        <v>1.1582531064373069</v>
       </c>
       <c r="T4" s="12">
         <f>INDEX('AEO 2020 47'!74:74,MATCH(T$1,'AEO 2020 47'!1:1,0))/INDEX('AEO 2019 48'!74:74,MATCH($B$1,'AEO 2019 48'!1:1,0))</f>
-        <v>1.1608925726874912</v>
+        <v>1.1566139492066752</v>
       </c>
       <c r="U4" s="12">
         <f>INDEX('AEO 2020 47'!74:74,MATCH(U$1,'AEO 2020 47'!1:1,0))/INDEX('AEO 2019 48'!74:74,MATCH($B$1,'AEO 2019 48'!1:1,0))</f>
-        <v>1.1587076742857145</v>
+        <v>1.1608925726874912</v>
       </c>
       <c r="V4" s="12">
         <f>INDEX('AEO 2020 47'!74:74,MATCH(V$1,'AEO 2020 47'!1:1,0))/INDEX('AEO 2019 48'!74:74,MATCH($B$1,'AEO 2019 48'!1:1,0))</f>
-        <v>1.1577974129923225</v>
+        <v>1.1587076742857145</v>
       </c>
       <c r="W4" s="12">
         <f>INDEX('AEO 2020 47'!74:74,MATCH(W$1,'AEO 2020 47'!1:1,0))/INDEX('AEO 2019 48'!74:74,MATCH($B$1,'AEO 2019 48'!1:1,0))</f>
-        <v>1.1595617134731571</v>
+        <v>1.1577974129923225</v>
       </c>
       <c r="X4" s="12">
         <f>INDEX('AEO 2020 47'!74:74,MATCH(X$1,'AEO 2020 47'!1:1,0))/INDEX('AEO 2019 48'!74:74,MATCH($B$1,'AEO 2019 48'!1:1,0))</f>
-        <v>1.1643668275375065</v>
+        <v>1.1595617134731571</v>
       </c>
       <c r="Y4" s="12">
         <f>INDEX('AEO 2020 47'!74:74,MATCH(Y$1,'AEO 2020 47'!1:1,0))/INDEX('AEO 2019 48'!74:74,MATCH($B$1,'AEO 2019 48'!1:1,0))</f>
-        <v>1.1639700403133857</v>
+        <v>1.1643668275375065</v>
       </c>
       <c r="Z4" s="12">
         <f>INDEX('AEO 2020 47'!74:74,MATCH(Z$1,'AEO 2020 47'!1:1,0))/INDEX('AEO 2019 48'!74:74,MATCH($B$1,'AEO 2019 48'!1:1,0))</f>
-        <v>1.1654091011063661</v>
+        <v>1.1639700403133857</v>
       </c>
       <c r="AA4" s="12">
         <f>INDEX('AEO 2020 47'!74:74,MATCH(AA$1,'AEO 2020 47'!1:1,0))/INDEX('AEO 2019 48'!74:74,MATCH($B$1,'AEO 2019 48'!1:1,0))</f>
-        <v>1.1654949927836271</v>
+        <v>1.1654091011063661</v>
       </c>
       <c r="AB4" s="12">
         <f>INDEX('AEO 2020 47'!74:74,MATCH(AB$1,'AEO 2020 47'!1:1,0))/INDEX('AEO 2019 48'!74:74,MATCH($B$1,'AEO 2019 48'!1:1,0))</f>
-        <v>1.1645674146198197</v>
+        <v>1.1654949927836271</v>
       </c>
       <c r="AC4" s="12">
         <f>INDEX('AEO 2020 47'!74:74,MATCH(AC$1,'AEO 2020 47'!1:1,0))/INDEX('AEO 2019 48'!74:74,MATCH($B$1,'AEO 2019 48'!1:1,0))</f>
-        <v>1.1556948563093714</v>
+        <v>1.1645674146198197</v>
       </c>
       <c r="AD4" s="12">
         <f>INDEX('AEO 2020 47'!74:74,MATCH(AD$1,'AEO 2020 47'!1:1,0))/INDEX('AEO 2019 48'!74:74,MATCH($B$1,'AEO 2019 48'!1:1,0))</f>
-        <v>1.156882158667961</v>
+        <v>1.1556948563093714</v>
       </c>
       <c r="AE4" s="12">
         <f>INDEX('AEO 2020 47'!74:74,MATCH(AE$1,'AEO 2020 47'!1:1,0))/INDEX('AEO 2019 48'!74:74,MATCH($B$1,'AEO 2019 48'!1:1,0))</f>
-        <v>1.1577308007641243</v>
+        <v>1.156882158667961</v>
       </c>
       <c r="AF4" s="12">
         <f>INDEX('AEO 2020 47'!74:74,MATCH(AF$1,'AEO 2020 47'!1:1,0))/INDEX('AEO 2019 48'!74:74,MATCH($B$1,'AEO 2019 48'!1:1,0))</f>
-        <v>1.1554726808619402</v>
+        <v>1.1577308007641243</v>
       </c>
       <c r="AG4" s="12">
         <f>INDEX('AEO 2020 47'!74:74,MATCH(AG$1,'AEO 2020 47'!1:1,0))/INDEX('AEO 2019 48'!74:74,MATCH($B$1,'AEO 2019 48'!1:1,0))</f>
+        <v>1.1554726808619402</v>
+      </c>
+      <c r="AH4" s="12">
+        <f>INDEX('AEO 2020 47'!74:74,MATCH(AH$1,'AEO 2020 47'!1:1,0))/INDEX('AEO 2019 48'!74:74,MATCH($B$1,'AEO 2019 48'!1:1,0))</f>
         <v>1.1425217975384818</v>
       </c>
-      <c r="AH4" s="12"/>
       <c r="AI4" s="12"/>
-    </row>
-    <row r="5" spans="1:35">
+      <c r="AJ4" s="12"/>
+    </row>
+    <row r="5" spans="1:36">
       <c r="A5" t="s">
         <v>373</v>
       </c>
@@ -71782,128 +71761,132 @@
       </c>
       <c r="D5" s="12">
         <f>INDEX('AEO 2020 7'!27:27,MATCH(D$1,'AEO 2020 7'!1:1,0))/INDEX('AEO 2019 7'!27:27,MATCH($B$1,'AEO 2019 7'!1:1,0))</f>
-        <v>0.92677369942698451</v>
+        <v>0.9605836299647178</v>
       </c>
       <c r="E5" s="12">
         <f>INDEX('AEO 2020 7'!27:27,MATCH(E$1,'AEO 2020 7'!1:1,0))/INDEX('AEO 2019 7'!27:27,MATCH($B$1,'AEO 2019 7'!1:1,0))</f>
-        <v>0.92997263149451737</v>
+        <v>0.92677369942698451</v>
       </c>
       <c r="F5" s="12">
         <f>INDEX('AEO 2020 7'!27:27,MATCH(F$1,'AEO 2020 7'!1:1,0))/INDEX('AEO 2019 7'!27:27,MATCH($B$1,'AEO 2019 7'!1:1,0))</f>
-        <v>0.93341608143377519</v>
+        <v>0.92997263149451737</v>
       </c>
       <c r="G5" s="12">
         <f>INDEX('AEO 2020 7'!27:27,MATCH(G$1,'AEO 2020 7'!1:1,0))/INDEX('AEO 2019 7'!27:27,MATCH($B$1,'AEO 2019 7'!1:1,0))</f>
-        <v>0.93743216579878175</v>
+        <v>0.93341608143377519</v>
       </c>
       <c r="H5" s="12">
         <f>INDEX('AEO 2020 7'!27:27,MATCH(H$1,'AEO 2020 7'!1:1,0))/INDEX('AEO 2019 7'!27:27,MATCH($B$1,'AEO 2019 7'!1:1,0))</f>
-        <v>0.92722595166077493</v>
+        <v>0.93743216579878175</v>
       </c>
       <c r="I5" s="12">
         <f>INDEX('AEO 2020 7'!27:27,MATCH(I$1,'AEO 2020 7'!1:1,0))/INDEX('AEO 2019 7'!27:27,MATCH($B$1,'AEO 2019 7'!1:1,0))</f>
-        <v>0.94751267443370224</v>
+        <v>0.92722595166077493</v>
       </c>
       <c r="J5" s="12">
         <f>INDEX('AEO 2020 7'!27:27,MATCH(J$1,'AEO 2020 7'!1:1,0))/INDEX('AEO 2019 7'!27:27,MATCH($B$1,'AEO 2019 7'!1:1,0))</f>
-        <v>0.9495312603725462</v>
+        <v>0.94751267443370224</v>
       </c>
       <c r="K5" s="12">
         <f>INDEX('AEO 2020 7'!27:27,MATCH(K$1,'AEO 2020 7'!1:1,0))/INDEX('AEO 2019 7'!27:27,MATCH($B$1,'AEO 2019 7'!1:1,0))</f>
-        <v>0.95154827648807061</v>
+        <v>0.9495312603725462</v>
       </c>
       <c r="L5" s="12">
         <f>INDEX('AEO 2020 7'!27:27,MATCH(L$1,'AEO 2020 7'!1:1,0))/INDEX('AEO 2019 7'!27:27,MATCH($B$1,'AEO 2019 7'!1:1,0))</f>
-        <v>0.96015587714949124</v>
+        <v>0.95154827648807061</v>
       </c>
       <c r="M5" s="12">
         <f>INDEX('AEO 2020 7'!27:27,MATCH(M$1,'AEO 2020 7'!1:1,0))/INDEX('AEO 2019 7'!27:27,MATCH($B$1,'AEO 2019 7'!1:1,0))</f>
-        <v>0.96139006799441495</v>
+        <v>0.96015587714949124</v>
       </c>
       <c r="N5" s="12">
         <f>INDEX('AEO 2020 7'!27:27,MATCH(N$1,'AEO 2020 7'!1:1,0))/INDEX('AEO 2019 7'!27:27,MATCH($B$1,'AEO 2019 7'!1:1,0))</f>
-        <v>0.96821554797650422</v>
+        <v>0.96139006799441495</v>
       </c>
       <c r="O5" s="12">
         <f>INDEX('AEO 2020 7'!27:27,MATCH(O$1,'AEO 2020 7'!1:1,0))/INDEX('AEO 2019 7'!27:27,MATCH($B$1,'AEO 2019 7'!1:1,0))</f>
-        <v>0.97260977191938602</v>
+        <v>0.96821554797650422</v>
       </c>
       <c r="P5" s="12">
         <f>INDEX('AEO 2020 7'!27:27,MATCH(P$1,'AEO 2020 7'!1:1,0))/INDEX('AEO 2019 7'!27:27,MATCH($B$1,'AEO 2019 7'!1:1,0))</f>
-        <v>0.97968017900064697</v>
+        <v>0.97260977191938602</v>
       </c>
       <c r="Q5" s="12">
         <f>INDEX('AEO 2020 7'!27:27,MATCH(Q$1,'AEO 2020 7'!1:1,0))/INDEX('AEO 2019 7'!27:27,MATCH($B$1,'AEO 2019 7'!1:1,0))</f>
-        <v>0.98510201946320619</v>
+        <v>0.97968017900064697</v>
       </c>
       <c r="R5" s="12">
         <f>INDEX('AEO 2020 7'!27:27,MATCH(R$1,'AEO 2020 7'!1:1,0))/INDEX('AEO 2019 7'!27:27,MATCH($B$1,'AEO 2019 7'!1:1,0))</f>
-        <v>0.98596250626380744</v>
+        <v>0.98510201946320619</v>
       </c>
       <c r="S5" s="12">
         <f>INDEX('AEO 2020 7'!27:27,MATCH(S$1,'AEO 2020 7'!1:1,0))/INDEX('AEO 2019 7'!27:27,MATCH($B$1,'AEO 2019 7'!1:1,0))</f>
-        <v>0.98981384974700415</v>
+        <v>0.98596250626380744</v>
       </c>
       <c r="T5" s="12">
         <f>INDEX('AEO 2020 7'!27:27,MATCH(T$1,'AEO 2020 7'!1:1,0))/INDEX('AEO 2019 7'!27:27,MATCH($B$1,'AEO 2019 7'!1:1,0))</f>
-        <v>0.98550718314700658</v>
+        <v>0.98981384974700415</v>
       </c>
       <c r="U5" s="12">
         <f>INDEX('AEO 2020 7'!27:27,MATCH(U$1,'AEO 2020 7'!1:1,0))/INDEX('AEO 2019 7'!27:27,MATCH($B$1,'AEO 2019 7'!1:1,0))</f>
-        <v>0.9865981298502482</v>
+        <v>0.98550718314700658</v>
       </c>
       <c r="V5" s="12">
         <f>INDEX('AEO 2020 7'!27:27,MATCH(V$1,'AEO 2020 7'!1:1,0))/INDEX('AEO 2019 7'!27:27,MATCH($B$1,'AEO 2019 7'!1:1,0))</f>
-        <v>0.98516384802802537</v>
+        <v>0.9865981298502482</v>
       </c>
       <c r="W5" s="12">
         <f>INDEX('AEO 2020 7'!27:27,MATCH(W$1,'AEO 2020 7'!1:1,0))/INDEX('AEO 2019 7'!27:27,MATCH($B$1,'AEO 2019 7'!1:1,0))</f>
-        <v>0.99189801829752966</v>
+        <v>0.98516384802802537</v>
       </c>
       <c r="X5" s="12">
         <f>INDEX('AEO 2020 7'!27:27,MATCH(X$1,'AEO 2020 7'!1:1,0))/INDEX('AEO 2019 7'!27:27,MATCH($B$1,'AEO 2019 7'!1:1,0))</f>
-        <v>0.9984778203710748</v>
+        <v>0.99189801829752966</v>
       </c>
       <c r="Y5" s="12">
         <f>INDEX('AEO 2020 7'!27:27,MATCH(Y$1,'AEO 2020 7'!1:1,0))/INDEX('AEO 2019 7'!27:27,MATCH($B$1,'AEO 2019 7'!1:1,0))</f>
-        <v>1.0048128999591717</v>
+        <v>0.9984778203710748</v>
       </c>
       <c r="Z5" s="12">
         <f>INDEX('AEO 2020 7'!27:27,MATCH(Z$1,'AEO 2020 7'!1:1,0))/INDEX('AEO 2019 7'!27:27,MATCH($B$1,'AEO 2019 7'!1:1,0))</f>
-        <v>1.0113845812159297</v>
+        <v>1.0048128999591717</v>
       </c>
       <c r="AA5" s="12">
         <f>INDEX('AEO 2020 7'!27:27,MATCH(AA$1,'AEO 2020 7'!1:1,0))/INDEX('AEO 2019 7'!27:27,MATCH($B$1,'AEO 2019 7'!1:1,0))</f>
-        <v>1.0199409993757336</v>
+        <v>1.0113845812159297</v>
       </c>
       <c r="AB5" s="12">
         <f>INDEX('AEO 2020 7'!27:27,MATCH(AB$1,'AEO 2020 7'!1:1,0))/INDEX('AEO 2019 7'!27:27,MATCH($B$1,'AEO 2019 7'!1:1,0))</f>
-        <v>1.0259134307692106</v>
+        <v>1.0199409993757336</v>
       </c>
       <c r="AC5" s="12">
         <f>INDEX('AEO 2020 7'!27:27,MATCH(AC$1,'AEO 2020 7'!1:1,0))/INDEX('AEO 2019 7'!27:27,MATCH($B$1,'AEO 2019 7'!1:1,0))</f>
-        <v>1.0354339300923505</v>
+        <v>1.0259134307692106</v>
       </c>
       <c r="AD5" s="12">
         <f>INDEX('AEO 2020 7'!27:27,MATCH(AD$1,'AEO 2020 7'!1:1,0))/INDEX('AEO 2019 7'!27:27,MATCH($B$1,'AEO 2019 7'!1:1,0))</f>
-        <v>1.0429859347050729</v>
+        <v>1.0354339300923505</v>
       </c>
       <c r="AE5" s="12">
         <f>INDEX('AEO 2020 7'!27:27,MATCH(AE$1,'AEO 2020 7'!1:1,0))/INDEX('AEO 2019 7'!27:27,MATCH($B$1,'AEO 2019 7'!1:1,0))</f>
-        <v>1.0511304324557778</v>
+        <v>1.0429859347050729</v>
       </c>
       <c r="AF5" s="12">
         <f>INDEX('AEO 2020 7'!27:27,MATCH(AF$1,'AEO 2020 7'!1:1,0))/INDEX('AEO 2019 7'!27:27,MATCH($B$1,'AEO 2019 7'!1:1,0))</f>
-        <v>1.0600172195977227</v>
+        <v>1.0511304324557778</v>
       </c>
       <c r="AG5" s="12">
         <f>INDEX('AEO 2020 7'!27:27,MATCH(AG$1,'AEO 2020 7'!1:1,0))/INDEX('AEO 2019 7'!27:27,MATCH($B$1,'AEO 2019 7'!1:1,0))</f>
+        <v>1.0600172195977227</v>
+      </c>
+      <c r="AH5" s="12">
+        <f>INDEX('AEO 2020 7'!27:27,MATCH(AH$1,'AEO 2020 7'!1:1,0))/INDEX('AEO 2019 7'!27:27,MATCH($B$1,'AEO 2019 7'!1:1,0))</f>
         <v>1.0675131276251466</v>
       </c>
-      <c r="AH5" s="12"/>
       <c r="AI5" s="12"/>
-    </row>
-    <row r="6" spans="1:35">
+      <c r="AJ5" s="12"/>
+    </row>
+    <row r="6" spans="1:36">
       <c r="A6" t="s">
         <v>374</v>
       </c>
@@ -71912,133 +71895,137 @@
         <v>1</v>
       </c>
       <c r="C6" s="17">
-        <f>($G$6-$B$6)/COUNT($C$1:$G$1)+B6</f>
-        <v>0.9903785426543098</v>
+        <f>($H$6-$B$6)/COUNT($C$1:$H$1)+B6</f>
+        <v>0.99198211887859145</v>
       </c>
       <c r="D6" s="17">
-        <f>($G$6-$B$6)/COUNT($C$1:$G$1)+C6</f>
-        <v>0.9807570853086196</v>
+        <f t="shared" ref="D6:G6" si="0">($H$6-$B$6)/COUNT($C$1:$H$1)+C6</f>
+        <v>0.98396423775718289</v>
       </c>
       <c r="E6" s="17">
-        <f>($G$6-$B$6)/COUNT($C$1:$G$1)+D6</f>
-        <v>0.9711356279629294</v>
+        <f t="shared" si="0"/>
+        <v>0.97594635663577434</v>
       </c>
       <c r="F6" s="17">
-        <f t="shared" ref="F6" si="0">($G$6-$B$6)/COUNT($C$1:$G$1)+E6</f>
-        <v>0.96151417061723921</v>
-      </c>
-      <c r="G6" s="12">
-        <f>SUM(INDEX('AEO 2020 7'!$C$62:$AJ$63,0,MATCH(G$1,'AEO 2020 7'!$C$1:$AJ$1,0)))/SUM(INDEX('AEO 2019 7'!$C$62:$AJ$63,0,MATCH($B$1,'AEO 2019 7'!$C$1:$AJ$1,0)))</f>
-        <v>0.9518927132715489</v>
+        <f t="shared" si="0"/>
+        <v>0.96792847551436578</v>
+      </c>
+      <c r="G6" s="17">
+        <f t="shared" si="0"/>
+        <v>0.95991059439295723</v>
       </c>
       <c r="H6" s="12">
         <f>SUM(INDEX('AEO 2020 7'!$C$62:$AJ$63,0,MATCH(H$1,'AEO 2020 7'!$C$1:$AJ$1,0)))/SUM(INDEX('AEO 2019 7'!$C$62:$AJ$63,0,MATCH($B$1,'AEO 2019 7'!$C$1:$AJ$1,0)))</f>
-        <v>0.95246155611659411</v>
+        <v>0.9518927132715489</v>
       </c>
       <c r="I6" s="12">
         <f>SUM(INDEX('AEO 2020 7'!$C$62:$AJ$63,0,MATCH(I$1,'AEO 2020 7'!$C$1:$AJ$1,0)))/SUM(INDEX('AEO 2019 7'!$C$62:$AJ$63,0,MATCH($B$1,'AEO 2019 7'!$C$1:$AJ$1,0)))</f>
-        <v>0.94175642841879503</v>
+        <v>0.95246155611659411</v>
       </c>
       <c r="J6" s="12">
         <f>SUM(INDEX('AEO 2020 7'!$C$62:$AJ$63,0,MATCH(J$1,'AEO 2020 7'!$C$1:$AJ$1,0)))/SUM(INDEX('AEO 2019 7'!$C$62:$AJ$63,0,MATCH($B$1,'AEO 2019 7'!$C$1:$AJ$1,0)))</f>
-        <v>0.93639149842109015</v>
+        <v>0.94175642841879503</v>
       </c>
       <c r="K6" s="12">
         <f>SUM(INDEX('AEO 2020 7'!$C$62:$AJ$63,0,MATCH(K$1,'AEO 2020 7'!$C$1:$AJ$1,0)))/SUM(INDEX('AEO 2019 7'!$C$62:$AJ$63,0,MATCH($B$1,'AEO 2019 7'!$C$1:$AJ$1,0)))</f>
-        <v>0.92080025800732879</v>
+        <v>0.93639149842109015</v>
       </c>
       <c r="L6" s="12">
         <f>SUM(INDEX('AEO 2020 7'!$C$62:$AJ$63,0,MATCH(L$1,'AEO 2020 7'!$C$1:$AJ$1,0)))/SUM(INDEX('AEO 2019 7'!$C$62:$AJ$63,0,MATCH($B$1,'AEO 2019 7'!$C$1:$AJ$1,0)))</f>
-        <v>0.9182518420615261</v>
+        <v>0.92080025800732879</v>
       </c>
       <c r="M6" s="12">
         <f>SUM(INDEX('AEO 2020 7'!$C$62:$AJ$63,0,MATCH(M$1,'AEO 2020 7'!$C$1:$AJ$1,0)))/SUM(INDEX('AEO 2019 7'!$C$62:$AJ$63,0,MATCH($B$1,'AEO 2019 7'!$C$1:$AJ$1,0)))</f>
-        <v>0.93156968967891551</v>
+        <v>0.9182518420615261</v>
       </c>
       <c r="N6" s="12">
         <f>SUM(INDEX('AEO 2020 7'!$C$62:$AJ$63,0,MATCH(N$1,'AEO 2020 7'!$C$1:$AJ$1,0)))/SUM(INDEX('AEO 2019 7'!$C$62:$AJ$63,0,MATCH($B$1,'AEO 2019 7'!$C$1:$AJ$1,0)))</f>
-        <v>0.92965540984385031</v>
+        <v>0.93156968967891551</v>
       </c>
       <c r="O6" s="12">
         <f>SUM(INDEX('AEO 2020 7'!$C$62:$AJ$63,0,MATCH(O$1,'AEO 2020 7'!$C$1:$AJ$1,0)))/SUM(INDEX('AEO 2019 7'!$C$62:$AJ$63,0,MATCH($B$1,'AEO 2019 7'!$C$1:$AJ$1,0)))</f>
-        <v>0.92834558736238948</v>
+        <v>0.92965540984385031</v>
       </c>
       <c r="P6" s="12">
         <f>SUM(INDEX('AEO 2020 7'!$C$62:$AJ$63,0,MATCH(P$1,'AEO 2020 7'!$C$1:$AJ$1,0)))/SUM(INDEX('AEO 2019 7'!$C$62:$AJ$63,0,MATCH($B$1,'AEO 2019 7'!$C$1:$AJ$1,0)))</f>
-        <v>0.9261068197826724</v>
+        <v>0.92834558736238948</v>
       </c>
       <c r="Q6" s="12">
         <f>SUM(INDEX('AEO 2020 7'!$C$62:$AJ$63,0,MATCH(Q$1,'AEO 2020 7'!$C$1:$AJ$1,0)))/SUM(INDEX('AEO 2019 7'!$C$62:$AJ$63,0,MATCH($B$1,'AEO 2019 7'!$C$1:$AJ$1,0)))</f>
-        <v>0.92484745118833744</v>
+        <v>0.9261068197826724</v>
       </c>
       <c r="R6" s="12">
         <f>SUM(INDEX('AEO 2020 7'!$C$62:$AJ$63,0,MATCH(R$1,'AEO 2020 7'!$C$1:$AJ$1,0)))/SUM(INDEX('AEO 2019 7'!$C$62:$AJ$63,0,MATCH($B$1,'AEO 2019 7'!$C$1:$AJ$1,0)))</f>
-        <v>0.92206853022880353</v>
+        <v>0.92484745118833744</v>
       </c>
       <c r="S6" s="12">
         <f>SUM(INDEX('AEO 2020 7'!$C$62:$AJ$63,0,MATCH(S$1,'AEO 2020 7'!$C$1:$AJ$1,0)))/SUM(INDEX('AEO 2019 7'!$C$62:$AJ$63,0,MATCH($B$1,'AEO 2019 7'!$C$1:$AJ$1,0)))</f>
-        <v>0.90758133958038201</v>
+        <v>0.92206853022880353</v>
       </c>
       <c r="T6" s="12">
         <f>SUM(INDEX('AEO 2020 7'!$C$62:$AJ$63,0,MATCH(T$1,'AEO 2020 7'!$C$1:$AJ$1,0)))/SUM(INDEX('AEO 2019 7'!$C$62:$AJ$63,0,MATCH($B$1,'AEO 2019 7'!$C$1:$AJ$1,0)))</f>
-        <v>0.90562550948533072</v>
+        <v>0.90758133958038201</v>
       </c>
       <c r="U6" s="12">
         <f>SUM(INDEX('AEO 2020 7'!$C$62:$AJ$63,0,MATCH(U$1,'AEO 2020 7'!$C$1:$AJ$1,0)))/SUM(INDEX('AEO 2019 7'!$C$62:$AJ$63,0,MATCH($B$1,'AEO 2019 7'!$C$1:$AJ$1,0)))</f>
-        <v>0.90075720402364812</v>
+        <v>0.90562550948533072</v>
       </c>
       <c r="V6" s="12">
         <f>SUM(INDEX('AEO 2020 7'!$C$62:$AJ$63,0,MATCH(V$1,'AEO 2020 7'!$C$1:$AJ$1,0)))/SUM(INDEX('AEO 2019 7'!$C$62:$AJ$63,0,MATCH($B$1,'AEO 2019 7'!$C$1:$AJ$1,0)))</f>
-        <v>0.89802379049171766</v>
+        <v>0.90075720402364812</v>
       </c>
       <c r="W6" s="12">
         <f>SUM(INDEX('AEO 2020 7'!$C$62:$AJ$63,0,MATCH(W$1,'AEO 2020 7'!$C$1:$AJ$1,0)))/SUM(INDEX('AEO 2019 7'!$C$62:$AJ$63,0,MATCH($B$1,'AEO 2019 7'!$C$1:$AJ$1,0)))</f>
-        <v>0.89379951405981661</v>
+        <v>0.89802379049171766</v>
       </c>
       <c r="X6" s="12">
         <f>SUM(INDEX('AEO 2020 7'!$C$62:$AJ$63,0,MATCH(X$1,'AEO 2020 7'!$C$1:$AJ$1,0)))/SUM(INDEX('AEO 2019 7'!$C$62:$AJ$63,0,MATCH($B$1,'AEO 2019 7'!$C$1:$AJ$1,0)))</f>
-        <v>0.89708000601489479</v>
+        <v>0.89379951405981661</v>
       </c>
       <c r="Y6" s="12">
         <f>SUM(INDEX('AEO 2020 7'!$C$62:$AJ$63,0,MATCH(Y$1,'AEO 2020 7'!$C$1:$AJ$1,0)))/SUM(INDEX('AEO 2019 7'!$C$62:$AJ$63,0,MATCH($B$1,'AEO 2019 7'!$C$1:$AJ$1,0)))</f>
-        <v>0.88961876647171034</v>
+        <v>0.89708000601489479</v>
       </c>
       <c r="Z6" s="12">
         <f>SUM(INDEX('AEO 2020 7'!$C$62:$AJ$63,0,MATCH(Z$1,'AEO 2020 7'!$C$1:$AJ$1,0)))/SUM(INDEX('AEO 2019 7'!$C$62:$AJ$63,0,MATCH($B$1,'AEO 2019 7'!$C$1:$AJ$1,0)))</f>
-        <v>0.88836335504499297</v>
+        <v>0.88961876647171034</v>
       </c>
       <c r="AA6" s="12">
         <f>SUM(INDEX('AEO 2020 7'!$C$62:$AJ$63,0,MATCH(AA$1,'AEO 2020 7'!$C$1:$AJ$1,0)))/SUM(INDEX('AEO 2019 7'!$C$62:$AJ$63,0,MATCH($B$1,'AEO 2019 7'!$C$1:$AJ$1,0)))</f>
-        <v>0.8828559670130508</v>
+        <v>0.88836335504499297</v>
       </c>
       <c r="AB6" s="12">
         <f>SUM(INDEX('AEO 2020 7'!$C$62:$AJ$63,0,MATCH(AB$1,'AEO 2020 7'!$C$1:$AJ$1,0)))/SUM(INDEX('AEO 2019 7'!$C$62:$AJ$63,0,MATCH($B$1,'AEO 2019 7'!$C$1:$AJ$1,0)))</f>
-        <v>0.88736219163771335</v>
+        <v>0.8828559670130508</v>
       </c>
       <c r="AC6" s="12">
         <f>SUM(INDEX('AEO 2020 7'!$C$62:$AJ$63,0,MATCH(AC$1,'AEO 2020 7'!$C$1:$AJ$1,0)))/SUM(INDEX('AEO 2019 7'!$C$62:$AJ$63,0,MATCH($B$1,'AEO 2019 7'!$C$1:$AJ$1,0)))</f>
-        <v>0.87973178317887191</v>
+        <v>0.88736219163771335</v>
       </c>
       <c r="AD6" s="12">
         <f>SUM(INDEX('AEO 2020 7'!$C$62:$AJ$63,0,MATCH(AD$1,'AEO 2020 7'!$C$1:$AJ$1,0)))/SUM(INDEX('AEO 2019 7'!$C$62:$AJ$63,0,MATCH($B$1,'AEO 2019 7'!$C$1:$AJ$1,0)))</f>
-        <v>0.87837744256171213</v>
+        <v>0.87973178317887191</v>
       </c>
       <c r="AE6" s="12">
         <f>SUM(INDEX('AEO 2020 7'!$C$62:$AJ$63,0,MATCH(AE$1,'AEO 2020 7'!$C$1:$AJ$1,0)))/SUM(INDEX('AEO 2019 7'!$C$62:$AJ$63,0,MATCH($B$1,'AEO 2019 7'!$C$1:$AJ$1,0)))</f>
-        <v>0.87723579970400389</v>
+        <v>0.87837744256171213</v>
       </c>
       <c r="AF6" s="12">
         <f>SUM(INDEX('AEO 2020 7'!$C$62:$AJ$63,0,MATCH(AF$1,'AEO 2020 7'!$C$1:$AJ$1,0)))/SUM(INDEX('AEO 2019 7'!$C$62:$AJ$63,0,MATCH($B$1,'AEO 2019 7'!$C$1:$AJ$1,0)))</f>
-        <v>0.87556389638552312</v>
+        <v>0.87723579970400389</v>
       </c>
       <c r="AG6" s="12">
         <f>SUM(INDEX('AEO 2020 7'!$C$62:$AJ$63,0,MATCH(AG$1,'AEO 2020 7'!$C$1:$AJ$1,0)))/SUM(INDEX('AEO 2019 7'!$C$62:$AJ$63,0,MATCH($B$1,'AEO 2019 7'!$C$1:$AJ$1,0)))</f>
+        <v>0.87556389638552312</v>
+      </c>
+      <c r="AH6" s="12">
+        <f>SUM(INDEX('AEO 2020 7'!$C$62:$AJ$63,0,MATCH(AH$1,'AEO 2020 7'!$C$1:$AJ$1,0)))/SUM(INDEX('AEO 2019 7'!$C$62:$AJ$63,0,MATCH($B$1,'AEO 2019 7'!$C$1:$AJ$1,0)))</f>
         <v>0.87350419064050711</v>
       </c>
-      <c r="AH6" s="12"/>
       <c r="AI6" s="12"/>
-    </row>
-    <row r="7" spans="1:35">
+      <c r="AJ6" s="12"/>
+    </row>
+    <row r="7" spans="1:36">
       <c r="A7" t="s">
         <v>375</v>
       </c>
@@ -72138,8 +72125,11 @@
       <c r="AG7" s="12">
         <v>0</v>
       </c>
-      <c r="AH7" s="12"/>
+      <c r="AH7" s="12">
+        <v>0</v>
+      </c>
       <c r="AI7" s="12"/>
+      <c r="AJ7" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>